<commit_message>
Updates to excel pin tables
</commit_message>
<xml_diff>
--- a/Pins for HoverBoard wheel.xlsx
+++ b/Pins for HoverBoard wheel.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29685" windowHeight="16470" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29685" windowHeight="16470" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
     <sheet name="Atmel Controler" sheetId="7" r:id="rId2"/>
-    <sheet name="Truth Table" sheetId="2" r:id="rId3"/>
-    <sheet name="Explore states" sheetId="4" r:id="rId4"/>
-    <sheet name="Sketch" sheetId="3" r:id="rId5"/>
-    <sheet name="3 Hall Synthesis" sheetId="5" r:id="rId6"/>
-    <sheet name="motor test" sheetId="6" r:id="rId7"/>
-    <sheet name="sin Pulse syntesis" sheetId="12" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId3"/>
+    <sheet name="Truth Table" sheetId="2" r:id="rId4"/>
+    <sheet name="Explore states" sheetId="4" r:id="rId5"/>
+    <sheet name="Sketch" sheetId="3" r:id="rId6"/>
+    <sheet name="3 Hall Synthesis" sheetId="5" r:id="rId7"/>
+    <sheet name="motor test" sheetId="6" r:id="rId8"/>
+    <sheet name="sin Pulse syntesis" sheetId="12" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="amplitude">'sin Pulse syntesis'!$H$2</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="291">
   <si>
     <t>Pin out</t>
   </si>
@@ -910,6 +911,33 @@
   </si>
   <si>
     <t>step</t>
+  </si>
+  <si>
+    <t>Cable pin #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pigtail </t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Accelreometers are connected via SPI</t>
+  </si>
+  <si>
+    <t>Logic Analizer interface</t>
+  </si>
+  <si>
+    <t>gnd</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1031,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1293,12 +1321,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1504,6 +1563,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5330,58 +5392,58 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="85"/>
                 <c:pt idx="0">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>-14</c:v>
@@ -5423,73 +5485,73 @@
                   <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-15</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>-14</c:v>
@@ -5531,58 +5593,58 @@
                   <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-13</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5914,73 +5976,73 @@
                   <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>-17</c:v>
@@ -6022,73 +6084,73 @@
                   <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-16</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>-17</c:v>
@@ -6130,22 +6192,22 @@
                   <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-18</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6456,22 +6518,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="85"/>
                 <c:pt idx="0">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-20</c:v>
@@ -6513,73 +6575,73 @@
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-19</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>-20</c:v>
@@ -6621,73 +6683,73 @@
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-21</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>-20</c:v>
@@ -9852,8 +9914,8 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>326102</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>2253</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>164178</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9912,7 +9974,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>495298</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>174493</xdr:rowOff>
+      <xdr:rowOff>136393</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11851,12 +11913,26 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29800C5-F2DC-491C-A496-777CBE6FE60C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B464C57-0DBE-40E5-955E-B8EBE134B27C}">
-  <dimension ref="A1:Y61"/>
+  <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13294,18 +13370,188 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="23:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="89" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" s="64" t="s">
+        <v>283</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="90">
+        <v>1</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C47" s="67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="90">
+        <v>2</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A49" s="90">
+        <v>3</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="67" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A50" s="90">
+        <v>4</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="67" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A51" s="90">
+        <v>5</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="67" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="91">
+        <v>6</v>
+      </c>
+      <c r="B52" s="71" t="s">
+        <v>284</v>
+      </c>
+      <c r="C52" s="72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A55" s="89">
+        <v>0</v>
+      </c>
+      <c r="B55" s="65" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A56" s="90">
+        <v>1</v>
+      </c>
+      <c r="B56" s="67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A57" s="90">
+        <v>2</v>
+      </c>
+      <c r="B57" s="67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A58" s="90">
+        <v>3</v>
+      </c>
+      <c r="B58" s="67" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A59" s="90">
+        <v>4</v>
+      </c>
+      <c r="B59" s="67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A60" s="90">
+        <v>5</v>
+      </c>
+      <c r="B60" s="67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A61" s="90">
+        <v>6</v>
+      </c>
+      <c r="B61" s="67" t="s">
+        <v>47</v>
+      </c>
       <c r="W61" t="s">
         <v>252</v>
       </c>
     </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A62" s="90">
+        <v>7</v>
+      </c>
+      <c r="B62" s="67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="91">
+        <v>8</v>
+      </c>
+      <c r="B63" s="72" t="s">
+        <v>223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12C6A90-4194-4CFA-A44E-A9C9B9CC903C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -14735,7 +14981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
@@ -16978,7 +17224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16993,13 +17239,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AT88"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <pane ySplit="15600" topLeftCell="A80"/>
-      <selection activeCell="AP22" sqref="AP22"/>
+      <selection activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="AH82" sqref="AH82"/>
     </sheetView>
   </sheetViews>
@@ -17031,7 +17277,7 @@
         <v>0</v>
       </c>
       <c r="S1">
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="AD1" s="24">
         <v>6</v>
@@ -17105,15 +17351,15 @@
       </c>
       <c r="S2">
         <f>I2+$S$1</f>
-        <v>90</v>
+        <v>-90</v>
       </c>
       <c r="T2">
         <f t="shared" ref="T2:U2" si="1">J2+$S$1</f>
-        <v>210</v>
+        <v>30</v>
       </c>
       <c r="U2">
         <f t="shared" si="1"/>
-        <v>330</v>
+        <v>150</v>
       </c>
       <c r="Y2">
         <f>Q2-5</f>
@@ -17298,19 +17544,19 @@
       </c>
       <c r="S4" s="41">
         <f t="shared" ref="S4:U19" si="7">SIN( ($A4+S$2)*deg2rad)</f>
-        <v>0.8660254037844386</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="T4" s="41">
         <f t="shared" si="7"/>
-        <v>1.22514845490862E-16</v>
+        <v>0</v>
       </c>
       <c r="U4" s="41">
         <f t="shared" si="7"/>
-        <v>-0.8660254037844386</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="V4">
         <f>IF(ABS(S4)&gt;0.5,1,0)*SIGN(S4)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W4">
         <f t="shared" ref="W4:W67" si="8">IF(ABS(T4)&gt;0.5,1,0)*SIGN(T4)</f>
@@ -17318,11 +17564,11 @@
       </c>
       <c r="X4">
         <f t="shared" ref="X4:X67" si="9">IF(ABS(U4)&gt;0.5,1,0)*SIGN(U4)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="41">
         <f>V4+Y$2</f>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z4" s="41">
         <f t="shared" ref="Z4:Z67" si="10">W4+Z$2</f>
@@ -17330,7 +17576,7 @@
       </c>
       <c r="AA4" s="41">
         <f t="shared" ref="AA4:AA67" si="11">X4+AA$2</f>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL4">
         <v>1</v>
@@ -17418,19 +17664,19 @@
       </c>
       <c r="S5" s="41">
         <f t="shared" si="7"/>
-        <v>0.90630778703664994</v>
+        <v>-0.90630778703665005</v>
       </c>
       <c r="T5" s="41">
         <f t="shared" si="7"/>
-        <v>-8.7155742747657944E-2</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="U5" s="41">
         <f t="shared" si="7"/>
-        <v>-0.8191520442889918</v>
+        <v>0.81915204428899169</v>
       </c>
       <c r="V5">
         <f t="shared" ref="V5:V68" si="20">IF(ABS(S5)&gt;0.5,1,0)*SIGN(S5)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W5">
         <f t="shared" si="8"/>
@@ -17438,11 +17684,11 @@
       </c>
       <c r="X5">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="41">
         <f t="shared" ref="Y5:Y68" si="21">V5+Y$2</f>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z5" s="41">
         <f t="shared" si="10"/>
@@ -17450,7 +17696,7 @@
       </c>
       <c r="AA5" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL5">
         <v>2</v>
@@ -17538,19 +17784,19 @@
       </c>
       <c r="S6" s="41">
         <f t="shared" si="7"/>
-        <v>0.93969262078590832</v>
+        <v>-0.93969262078590843</v>
       </c>
       <c r="T6" s="41">
         <f t="shared" si="7"/>
-        <v>-0.17364817766693047</v>
+        <v>0.17364817766693033</v>
       </c>
       <c r="U6" s="41">
         <f t="shared" si="7"/>
-        <v>-0.76604444311897812</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="V6">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W6">
         <f t="shared" si="8"/>
@@ -17558,11 +17804,11 @@
       </c>
       <c r="X6">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z6" s="41">
         <f t="shared" si="10"/>
@@ -17570,7 +17816,7 @@
       </c>
       <c r="AA6" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL6">
         <v>3</v>
@@ -17658,19 +17904,19 @@
       </c>
       <c r="S7" s="41">
         <f t="shared" si="7"/>
-        <v>0.96592582628906831</v>
+        <v>-0.96592582628906831</v>
       </c>
       <c r="T7" s="41">
         <f t="shared" si="7"/>
-        <v>-0.25881904510252079</v>
+        <v>0.25881904510252074</v>
       </c>
       <c r="U7" s="41">
         <f t="shared" si="7"/>
-        <v>-0.70710678118654768</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="V7">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W7">
         <f t="shared" si="8"/>
@@ -17678,11 +17924,11 @@
       </c>
       <c r="X7">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z7" s="41">
         <f t="shared" si="10"/>
@@ -17690,7 +17936,7 @@
       </c>
       <c r="AA7" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL7">
         <v>4</v>
@@ -17778,19 +18024,19 @@
       </c>
       <c r="S8" s="41">
         <f t="shared" si="7"/>
-        <v>0.98480775301220802</v>
+        <v>-0.98480775301220802</v>
       </c>
       <c r="T8" s="41">
         <f t="shared" si="7"/>
-        <v>-0.34202014332566866</v>
+        <v>0.34202014332566871</v>
       </c>
       <c r="U8" s="41">
         <f t="shared" si="7"/>
-        <v>-0.64278760968653958</v>
+        <v>0.64278760968653947</v>
       </c>
       <c r="V8">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W8">
         <f t="shared" si="8"/>
@@ -17798,11 +18044,11 @@
       </c>
       <c r="X8">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z8" s="41">
         <f t="shared" si="10"/>
@@ -17810,7 +18056,7 @@
       </c>
       <c r="AA8" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL8">
         <v>5</v>
@@ -17898,19 +18144,19 @@
       </c>
       <c r="S9" s="41">
         <f t="shared" si="7"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="T9" s="41">
         <f t="shared" si="7"/>
-        <v>-0.42261826174069927</v>
+        <v>0.42261826174069944</v>
       </c>
       <c r="U9" s="41">
         <f t="shared" si="7"/>
-        <v>-0.57357643635104649</v>
+        <v>0.57357643635104594</v>
       </c>
       <c r="V9">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W9">
         <f t="shared" si="8"/>
@@ -17918,11 +18164,11 @@
       </c>
       <c r="X9">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z9" s="41">
         <f t="shared" si="10"/>
@@ -17930,7 +18176,7 @@
       </c>
       <c r="AA9" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
       <c r="AL9">
         <v>6</v>
@@ -18018,19 +18264,19 @@
       </c>
       <c r="S10" s="41">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T10" s="41">
         <f t="shared" si="7"/>
-        <v>-0.50000000000000011</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="U10" s="41">
         <f t="shared" si="7"/>
-        <v>-0.50000000000000044</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="V10">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W10">
         <f t="shared" si="8"/>
@@ -18042,7 +18288,7 @@
       </c>
       <c r="Y10" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z10" s="41">
         <f t="shared" si="10"/>
@@ -18138,23 +18384,23 @@
       </c>
       <c r="S11" s="41">
         <f t="shared" si="7"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="T11" s="41">
         <f t="shared" si="7"/>
-        <v>-0.57357643635104616</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="U11" s="41">
         <f t="shared" si="7"/>
-        <v>-0.42261826174069922</v>
+        <v>0.4226182617406995</v>
       </c>
       <c r="V11">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W11">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X11">
         <f t="shared" si="9"/>
@@ -18162,11 +18408,11 @@
       </c>
       <c r="Y11" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z11" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA11" s="41">
         <f t="shared" si="11"/>
@@ -18240,23 +18486,23 @@
       </c>
       <c r="S12" s="41">
         <f t="shared" si="7"/>
-        <v>0.98480775301220802</v>
+        <v>-0.98480775301220802</v>
       </c>
       <c r="T12" s="41">
         <f t="shared" si="7"/>
-        <v>-0.64278760968653925</v>
+        <v>0.64278760968653925</v>
       </c>
       <c r="U12" s="41">
         <f t="shared" si="7"/>
-        <v>-0.3420201433256686</v>
+        <v>0.34202014332566888</v>
       </c>
       <c r="V12">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W12">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X12">
         <f t="shared" si="9"/>
@@ -18264,11 +18510,11 @@
       </c>
       <c r="Y12" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z12" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA12" s="41">
         <f t="shared" si="11"/>
@@ -18342,23 +18588,23 @@
       </c>
       <c r="S13" s="41">
         <f t="shared" si="7"/>
-        <v>0.96592582628906831</v>
+        <v>-0.96592582628906831</v>
       </c>
       <c r="T13" s="41">
         <f t="shared" si="7"/>
-        <v>-0.70710678118654746</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="U13" s="41">
         <f t="shared" si="7"/>
-        <v>-0.25881904510252068</v>
+        <v>0.25881904510252102</v>
       </c>
       <c r="V13">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W13">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X13">
         <f t="shared" si="9"/>
@@ -18366,11 +18612,11 @@
       </c>
       <c r="Y13" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z13" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA13" s="41">
         <f t="shared" si="11"/>
@@ -18450,23 +18696,23 @@
       </c>
       <c r="S14" s="41">
         <f t="shared" si="7"/>
-        <v>0.93969262078590843</v>
+        <v>-0.93969262078590832</v>
       </c>
       <c r="T14" s="41">
         <f t="shared" si="7"/>
-        <v>-0.7660444431189779</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="U14" s="41">
         <f t="shared" si="7"/>
-        <v>-0.17364817766693039</v>
+        <v>0.17364817766693028</v>
       </c>
       <c r="V14">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W14">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="9"/>
@@ -18474,11 +18720,11 @@
       </c>
       <c r="Y14" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z14" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA14" s="41">
         <f t="shared" si="11"/>
@@ -18566,23 +18812,23 @@
       </c>
       <c r="S15" s="41">
         <f t="shared" si="7"/>
-        <v>0.90630778703665005</v>
+        <v>-0.90630778703664994</v>
       </c>
       <c r="T15" s="41">
         <f t="shared" si="7"/>
-        <v>-0.81915204428899158</v>
+        <v>0.8191520442889918</v>
       </c>
       <c r="U15" s="41">
         <f t="shared" si="7"/>
-        <v>-8.7155742747658319E-2</v>
+        <v>8.7155742747658194E-2</v>
       </c>
       <c r="V15">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W15">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X15">
         <f t="shared" si="9"/>
@@ -18590,11 +18836,11 @@
       </c>
       <c r="Y15" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z15" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA15" s="41">
         <f t="shared" si="11"/>
@@ -18680,23 +18926,23 @@
       </c>
       <c r="S16" s="41">
         <f t="shared" si="7"/>
-        <v>0.86602540378443871</v>
+        <v>-0.8660254037844386</v>
       </c>
       <c r="T16" s="41">
         <f t="shared" si="7"/>
-        <v>-0.86602540378443837</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="U16" s="41">
         <f t="shared" si="7"/>
-        <v>-2.45029690981724E-16</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="V16">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W16">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X16">
         <f t="shared" si="9"/>
@@ -18704,11 +18950,11 @@
       </c>
       <c r="Y16" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z16" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA16" s="41">
         <f t="shared" si="11"/>
@@ -18801,23 +19047,23 @@
       </c>
       <c r="S17" s="41">
         <f t="shared" si="7"/>
-        <v>0.81915204428899169</v>
+        <v>-0.8191520442889918</v>
       </c>
       <c r="T17" s="41">
         <f t="shared" si="7"/>
-        <v>-0.90630778703665005</v>
+        <v>0.90630778703664994</v>
       </c>
       <c r="U17" s="41">
         <f t="shared" si="7"/>
-        <v>8.7155742747657833E-2</v>
+        <v>-8.7155742747657944E-2</v>
       </c>
       <c r="V17">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W17">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X17">
         <f t="shared" si="9"/>
@@ -18825,11 +19071,11 @@
       </c>
       <c r="Y17" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z17" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA17" s="41">
         <f t="shared" si="11"/>
@@ -18922,23 +19168,23 @@
       </c>
       <c r="S18" s="41">
         <f t="shared" si="7"/>
-        <v>0.76604444311897801</v>
+        <v>-0.76604444311897801</v>
       </c>
       <c r="T18" s="41">
         <f t="shared" si="7"/>
-        <v>-0.93969262078590843</v>
+        <v>0.93969262078590832</v>
       </c>
       <c r="U18" s="41">
         <f t="shared" si="7"/>
-        <v>0.17364817766692991</v>
+        <v>-0.17364817766693047</v>
       </c>
       <c r="V18">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W18">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X18">
         <f t="shared" si="9"/>
@@ -18946,11 +19192,11 @@
       </c>
       <c r="Y18" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z18" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA18" s="41">
         <f t="shared" si="11"/>
@@ -19043,23 +19289,23 @@
       </c>
       <c r="S19" s="41">
         <f t="shared" si="7"/>
-        <v>0.70710678118654757</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="T19" s="41">
         <f t="shared" si="7"/>
-        <v>-0.96592582628906831</v>
+        <v>0.96592582628906831</v>
       </c>
       <c r="U19" s="41">
         <f t="shared" si="7"/>
-        <v>0.25881904510252024</v>
+        <v>-0.25881904510252079</v>
       </c>
       <c r="V19">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W19">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X19">
         <f t="shared" si="9"/>
@@ -19067,11 +19313,11 @@
       </c>
       <c r="Y19" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z19" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA19" s="41">
         <f t="shared" si="11"/>
@@ -19164,23 +19410,23 @@
       </c>
       <c r="S20" s="41">
         <f t="shared" ref="S20:U83" si="30">SIN( ($A20+S$2)*deg2rad)</f>
-        <v>0.64278760968653947</v>
+        <v>-0.64278760968653925</v>
       </c>
       <c r="T20" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220802</v>
+        <v>0.98480775301220802</v>
       </c>
       <c r="U20" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566893</v>
+        <v>-0.34202014332566866</v>
       </c>
       <c r="V20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W20">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X20">
         <f t="shared" si="9"/>
@@ -19188,11 +19434,11 @@
       </c>
       <c r="Y20" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z20" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA20" s="41">
         <f t="shared" si="11"/>
@@ -19285,23 +19531,23 @@
       </c>
       <c r="S21" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104594</v>
+        <v>-0.57357643635104605</v>
       </c>
       <c r="T21" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="U21" s="41">
         <f t="shared" si="30"/>
-        <v>0.42261826174069955</v>
+        <v>-0.42261826174069927</v>
       </c>
       <c r="V21">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W21">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X21">
         <f t="shared" si="9"/>
@@ -19309,11 +19555,11 @@
       </c>
       <c r="Y21" s="41">
         <f t="shared" si="21"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z21" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA21" s="41">
         <f t="shared" si="11"/>
@@ -19406,15 +19652,15 @@
       </c>
       <c r="S22" s="41">
         <f t="shared" si="30"/>
-        <v>0.49999999999999994</v>
+        <v>-0.49999999999999994</v>
       </c>
       <c r="T22" s="41">
         <f t="shared" si="30"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U22" s="41">
         <f t="shared" si="30"/>
-        <v>0.5</v>
+        <v>-0.50000000000000011</v>
       </c>
       <c r="V22">
         <f t="shared" si="20"/>
@@ -19422,7 +19668,7 @@
       </c>
       <c r="W22">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X22">
         <f t="shared" si="9"/>
@@ -19434,7 +19680,7 @@
       </c>
       <c r="Z22" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA22" s="41">
         <f t="shared" si="11"/>
@@ -19526,15 +19772,15 @@
       </c>
       <c r="S23" s="41">
         <f t="shared" si="30"/>
-        <v>0.4226182617406995</v>
+        <v>-0.42261826174069944</v>
       </c>
       <c r="T23" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="U23" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104605</v>
+        <v>-0.57357643635104616</v>
       </c>
       <c r="V23">
         <f t="shared" si="20"/>
@@ -19542,11 +19788,11 @@
       </c>
       <c r="W23">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X23">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y23" s="41">
         <f t="shared" si="21"/>
@@ -19554,11 +19800,11 @@
       </c>
       <c r="Z23" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA23" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
@@ -19628,15 +19874,15 @@
       </c>
       <c r="S24" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566888</v>
+        <v>-0.34202014332566871</v>
       </c>
       <c r="T24" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220813</v>
+        <v>0.98480775301220802</v>
       </c>
       <c r="U24" s="41">
         <f t="shared" si="30"/>
-        <v>0.64278760968653914</v>
+        <v>-0.64278760968653925</v>
       </c>
       <c r="V24">
         <f t="shared" si="20"/>
@@ -19644,11 +19890,11 @@
       </c>
       <c r="W24">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X24">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y24" s="41">
         <f t="shared" si="21"/>
@@ -19656,11 +19902,11 @@
       </c>
       <c r="Z24" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA24" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AM24" t="s">
         <v>265</v>
@@ -19739,15 +19985,15 @@
       </c>
       <c r="S25" s="41">
         <f t="shared" si="30"/>
-        <v>0.25881904510252102</v>
+        <v>-0.25881904510252074</v>
       </c>
       <c r="T25" s="41">
         <f t="shared" si="30"/>
-        <v>-0.96592582628906842</v>
+        <v>0.96592582628906831</v>
       </c>
       <c r="U25" s="41">
         <f t="shared" si="30"/>
-        <v>0.70710678118654735</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="V25">
         <f t="shared" si="20"/>
@@ -19755,11 +20001,11 @@
       </c>
       <c r="W25">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X25">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y25" s="41">
         <f t="shared" si="21"/>
@@ -19767,11 +20013,11 @@
       </c>
       <c r="Z25" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA25" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK25" t="s">
         <v>262</v>
@@ -19868,15 +20114,15 @@
       </c>
       <c r="S26" s="41">
         <f t="shared" si="30"/>
-        <v>0.17364817766693028</v>
+        <v>-0.17364817766693033</v>
       </c>
       <c r="T26" s="41">
         <f t="shared" si="30"/>
-        <v>-0.93969262078590832</v>
+        <v>0.93969262078590843</v>
       </c>
       <c r="U26" s="41">
         <f t="shared" si="30"/>
-        <v>0.76604444311897779</v>
+        <v>-0.7660444431189779</v>
       </c>
       <c r="V26">
         <f t="shared" si="20"/>
@@ -19884,11 +20130,11 @@
       </c>
       <c r="W26">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X26">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y26" s="41">
         <f t="shared" si="21"/>
@@ -19896,11 +20142,11 @@
       </c>
       <c r="Z26" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA26" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK26">
         <v>704</v>
@@ -20000,15 +20246,15 @@
       </c>
       <c r="S27" s="41">
         <f t="shared" si="30"/>
-        <v>8.7155742747658194E-2</v>
+        <v>-8.7155742747658166E-2</v>
       </c>
       <c r="T27" s="41">
         <f t="shared" si="30"/>
-        <v>-0.90630778703664994</v>
+        <v>0.90630778703665005</v>
       </c>
       <c r="U27" s="41">
         <f t="shared" si="30"/>
-        <v>0.81915204428899147</v>
+        <v>-0.81915204428899158</v>
       </c>
       <c r="V27">
         <f t="shared" si="20"/>
@@ -20016,11 +20262,11 @@
       </c>
       <c r="W27">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X27">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y27" s="41">
         <f t="shared" si="21"/>
@@ -20028,11 +20274,11 @@
       </c>
       <c r="Z27" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA27" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK27">
         <v>576</v>
@@ -20132,15 +20378,15 @@
       </c>
       <c r="S28" s="41">
         <f t="shared" si="30"/>
-        <v>1.22514845490862E-16</v>
+        <v>0</v>
       </c>
       <c r="T28" s="41">
         <f t="shared" si="30"/>
-        <v>-0.8660254037844386</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="U28" s="41">
         <f t="shared" si="30"/>
-        <v>0.86602540378443882</v>
+        <v>-0.86602540378443837</v>
       </c>
       <c r="V28">
         <f t="shared" si="20"/>
@@ -20148,11 +20394,11 @@
       </c>
       <c r="W28">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X28">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y28" s="41">
         <f t="shared" si="21"/>
@@ -20160,11 +20406,11 @@
       </c>
       <c r="Z28" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA28" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK28">
         <v>448</v>
@@ -20264,15 +20510,15 @@
       </c>
       <c r="S29" s="41">
         <f t="shared" si="30"/>
-        <v>-8.7155742747657944E-2</v>
+        <v>8.7155742747658166E-2</v>
       </c>
       <c r="T29" s="41">
         <f t="shared" si="30"/>
-        <v>-0.8191520442889918</v>
+        <v>0.81915204428899169</v>
       </c>
       <c r="U29" s="41">
         <f t="shared" si="30"/>
-        <v>0.90630778703665005</v>
+        <v>-0.90630778703665005</v>
       </c>
       <c r="V29">
         <f t="shared" si="20"/>
@@ -20280,11 +20526,11 @@
       </c>
       <c r="W29">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X29">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y29" s="41">
         <f t="shared" si="21"/>
@@ -20292,11 +20538,11 @@
       </c>
       <c r="Z29" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA29" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK29">
         <v>320</v>
@@ -20396,15 +20642,15 @@
       </c>
       <c r="S30" s="41">
         <f t="shared" si="30"/>
-        <v>-0.17364817766693047</v>
+        <v>0.17364817766693033</v>
       </c>
       <c r="T30" s="41">
         <f t="shared" si="30"/>
-        <v>-0.76604444311897812</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="U30" s="41">
         <f t="shared" si="30"/>
-        <v>0.93969262078590843</v>
+        <v>-0.93969262078590843</v>
       </c>
       <c r="V30">
         <f t="shared" si="20"/>
@@ -20412,11 +20658,11 @@
       </c>
       <c r="W30">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X30">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y30" s="41">
         <f t="shared" si="21"/>
@@ -20424,11 +20670,11 @@
       </c>
       <c r="Z30" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA30" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK30">
         <v>192</v>
@@ -20528,15 +20774,15 @@
       </c>
       <c r="S31" s="41">
         <f t="shared" si="30"/>
-        <v>-0.25881904510252079</v>
+        <v>0.25881904510252074</v>
       </c>
       <c r="T31" s="41">
         <f t="shared" si="30"/>
-        <v>-0.70710678118654768</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="U31" s="41">
         <f t="shared" si="30"/>
-        <v>0.96592582628906831</v>
+        <v>-0.96592582628906831</v>
       </c>
       <c r="V31">
         <f t="shared" si="20"/>
@@ -20544,11 +20790,11 @@
       </c>
       <c r="W31">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X31">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y31" s="41">
         <f t="shared" si="21"/>
@@ -20556,11 +20802,11 @@
       </c>
       <c r="Z31" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA31" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AK31">
         <v>64</v>
@@ -20660,15 +20906,15 @@
       </c>
       <c r="S32" s="41">
         <f t="shared" si="30"/>
-        <v>-0.34202014332566866</v>
+        <v>0.34202014332566871</v>
       </c>
       <c r="T32" s="41">
         <f t="shared" si="30"/>
-        <v>-0.64278760968653958</v>
+        <v>0.64278760968653947</v>
       </c>
       <c r="U32" s="41">
         <f t="shared" si="30"/>
-        <v>0.98480775301220802</v>
+        <v>-0.98480775301220802</v>
       </c>
       <c r="V32">
         <f t="shared" si="20"/>
@@ -20676,11 +20922,11 @@
       </c>
       <c r="W32">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X32">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y32" s="41">
         <f t="shared" si="21"/>
@@ -20688,11 +20934,11 @@
       </c>
       <c r="Z32" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA32" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="33" spans="1:42" x14ac:dyDescent="0.25">
@@ -20762,15 +21008,15 @@
       </c>
       <c r="S33" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069927</v>
+        <v>0.42261826174069944</v>
       </c>
       <c r="T33" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104649</v>
+        <v>0.57357643635104594</v>
       </c>
       <c r="U33" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="V33">
         <f t="shared" si="20"/>
@@ -20778,11 +21024,11 @@
       </c>
       <c r="W33">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X33">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y33" s="41">
         <f t="shared" si="21"/>
@@ -20790,11 +21036,11 @@
       </c>
       <c r="Z33" s="41">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA33" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.25">
@@ -20864,15 +21110,15 @@
       </c>
       <c r="S34" s="41">
         <f t="shared" si="30"/>
-        <v>-0.50000000000000011</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="T34" s="41">
         <f t="shared" si="30"/>
-        <v>-0.50000000000000044</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="U34" s="41">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V34">
         <f t="shared" si="20"/>
@@ -20884,7 +21130,7 @@
       </c>
       <c r="X34">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y34" s="41">
         <f t="shared" si="21"/>
@@ -20896,7 +21142,7 @@
       </c>
       <c r="AA34" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.25">
@@ -20966,19 +21212,19 @@
       </c>
       <c r="S35" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104616</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="T35" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069922</v>
+        <v>0.4226182617406995</v>
       </c>
       <c r="U35" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="V35">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W35">
         <f t="shared" si="8"/>
@@ -20986,11 +21232,11 @@
       </c>
       <c r="X35">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y35" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z35" s="41">
         <f t="shared" si="10"/>
@@ -20998,7 +21244,7 @@
       </c>
       <c r="AA35" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.25">
@@ -21068,19 +21314,19 @@
       </c>
       <c r="S36" s="41">
         <f t="shared" si="30"/>
-        <v>-0.64278760968653925</v>
+        <v>0.64278760968653925</v>
       </c>
       <c r="T36" s="41">
         <f t="shared" si="30"/>
-        <v>-0.3420201433256686</v>
+        <v>0.34202014332566888</v>
       </c>
       <c r="U36" s="41">
         <f t="shared" si="30"/>
-        <v>0.98480775301220813</v>
+        <v>-0.98480775301220813</v>
       </c>
       <c r="V36">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W36">
         <f t="shared" si="8"/>
@@ -21088,11 +21334,11 @@
       </c>
       <c r="X36">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y36" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z36" s="41">
         <f t="shared" si="10"/>
@@ -21100,7 +21346,7 @@
       </c>
       <c r="AA36" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AN36" t="s">
         <v>264</v>
@@ -21176,19 +21422,19 @@
       </c>
       <c r="S37" s="41">
         <f t="shared" si="30"/>
-        <v>-0.70710678118654746</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="T37" s="41">
         <f t="shared" si="30"/>
-        <v>-0.25881904510252068</v>
+        <v>0.25881904510252102</v>
       </c>
       <c r="U37" s="41">
         <f t="shared" si="30"/>
-        <v>0.96592582628906842</v>
+        <v>-0.96592582628906842</v>
       </c>
       <c r="V37">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W37">
         <f t="shared" si="8"/>
@@ -21196,11 +21442,11 @@
       </c>
       <c r="X37">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y37" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z37" s="41">
         <f t="shared" si="10"/>
@@ -21208,7 +21454,7 @@
       </c>
       <c r="AA37" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AN37">
         <v>300</v>
@@ -21289,19 +21535,19 @@
       </c>
       <c r="S38" s="41">
         <f t="shared" si="30"/>
-        <v>-0.7660444431189779</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="T38" s="41">
         <f t="shared" si="30"/>
-        <v>-0.17364817766693039</v>
+        <v>0.17364817766693028</v>
       </c>
       <c r="U38" s="41">
         <f t="shared" si="30"/>
-        <v>0.93969262078590865</v>
+        <v>-0.93969262078590832</v>
       </c>
       <c r="V38">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W38">
         <f t="shared" si="8"/>
@@ -21309,11 +21555,11 @@
       </c>
       <c r="X38">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y38" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z38" s="41">
         <f t="shared" si="10"/>
@@ -21321,7 +21567,7 @@
       </c>
       <c r="AA38" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC38" s="43" t="s">
         <v>120</v>
@@ -21430,19 +21676,19 @@
       </c>
       <c r="S39" s="41">
         <f t="shared" si="30"/>
-        <v>-0.81915204428899158</v>
+        <v>0.8191520442889918</v>
       </c>
       <c r="T39" s="41">
         <f t="shared" si="30"/>
-        <v>-8.7155742747658319E-2</v>
+        <v>8.7155742747658194E-2</v>
       </c>
       <c r="U39" s="41">
         <f t="shared" si="30"/>
-        <v>0.90630778703665027</v>
+        <v>-0.90630778703664994</v>
       </c>
       <c r="V39">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W39">
         <f t="shared" si="8"/>
@@ -21450,11 +21696,11 @@
       </c>
       <c r="X39">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y39" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z39" s="41">
         <f t="shared" si="10"/>
@@ -21462,7 +21708,7 @@
       </c>
       <c r="AA39" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC39" t="s">
         <v>121</v>
@@ -21574,19 +21820,19 @@
       </c>
       <c r="S40" s="41">
         <f t="shared" si="30"/>
-        <v>-0.86602540378443837</v>
+        <v>0.8660254037844386</v>
       </c>
       <c r="T40" s="41">
         <f t="shared" si="30"/>
-        <v>-2.45029690981724E-16</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="U40" s="41">
         <f t="shared" si="30"/>
-        <v>0.86602540378443915</v>
+        <v>-0.8660254037844386</v>
       </c>
       <c r="V40">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W40">
         <f t="shared" si="8"/>
@@ -21594,11 +21840,11 @@
       </c>
       <c r="X40">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y40" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z40" s="41">
         <f t="shared" si="10"/>
@@ -21606,7 +21852,7 @@
       </c>
       <c r="AA40" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AL40">
         <v>2</v>
@@ -21694,19 +21940,19 @@
       </c>
       <c r="S41" s="41">
         <f t="shared" si="30"/>
-        <v>-0.90630778703665005</v>
+        <v>0.90630778703664994</v>
       </c>
       <c r="T41" s="41">
         <f t="shared" si="30"/>
-        <v>8.7155742747657833E-2</v>
+        <v>-8.7155742747657944E-2</v>
       </c>
       <c r="U41" s="41">
         <f t="shared" si="30"/>
-        <v>0.81915204428899235</v>
+        <v>-0.8191520442889918</v>
       </c>
       <c r="V41">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W41">
         <f t="shared" si="8"/>
@@ -21714,11 +21960,11 @@
       </c>
       <c r="X41">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y41" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z41" s="41">
         <f t="shared" si="10"/>
@@ -21726,7 +21972,7 @@
       </c>
       <c r="AA41" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AD41" t="s">
         <v>11</v>
@@ -21829,19 +22075,19 @@
       </c>
       <c r="S42" s="41">
         <f t="shared" si="30"/>
-        <v>-0.93969262078590843</v>
+        <v>0.93969262078590832</v>
       </c>
       <c r="T42" s="41">
         <f t="shared" si="30"/>
-        <v>0.17364817766692991</v>
+        <v>-0.17364817766693047</v>
       </c>
       <c r="U42" s="41">
         <f t="shared" si="30"/>
-        <v>0.76604444311897757</v>
+        <v>-0.76604444311897812</v>
       </c>
       <c r="V42">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W42">
         <f t="shared" si="8"/>
@@ -21849,11 +22095,11 @@
       </c>
       <c r="X42">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y42" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z42" s="41">
         <f t="shared" si="10"/>
@@ -21861,7 +22107,7 @@
       </c>
       <c r="AA42" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC42">
         <v>0</v>
@@ -21968,19 +22214,19 @@
       </c>
       <c r="S43" s="41">
         <f t="shared" si="30"/>
-        <v>-0.96592582628906831</v>
+        <v>0.96592582628906831</v>
       </c>
       <c r="T43" s="41">
         <f t="shared" si="30"/>
-        <v>0.25881904510252024</v>
+        <v>-0.25881904510252079</v>
       </c>
       <c r="U43" s="41">
         <f t="shared" si="30"/>
-        <v>0.70710678118654713</v>
+        <v>-0.70710678118654768</v>
       </c>
       <c r="V43">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W43">
         <f t="shared" si="8"/>
@@ -21988,11 +22234,11 @@
       </c>
       <c r="X43">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y43" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z43" s="41">
         <f t="shared" si="10"/>
@@ -22000,7 +22246,7 @@
       </c>
       <c r="AA43" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC43">
         <v>1</v>
@@ -22108,19 +22354,19 @@
       </c>
       <c r="S44" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220802</v>
+        <v>0.98480775301220802</v>
       </c>
       <c r="T44" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566893</v>
+        <v>-0.34202014332566866</v>
       </c>
       <c r="U44" s="41">
         <f t="shared" si="30"/>
-        <v>0.64278760968653903</v>
+        <v>-0.64278760968653958</v>
       </c>
       <c r="V44">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W44">
         <f t="shared" si="8"/>
@@ -22128,11 +22374,11 @@
       </c>
       <c r="X44">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y44" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z44" s="41">
         <f t="shared" si="10"/>
@@ -22140,7 +22386,7 @@
       </c>
       <c r="AA44" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC44">
         <v>2</v>
@@ -22248,19 +22494,19 @@
       </c>
       <c r="S45" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="T45" s="41">
         <f t="shared" si="30"/>
-        <v>0.42261826174069955</v>
+        <v>-0.42261826174069927</v>
       </c>
       <c r="U45" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104583</v>
+        <v>-0.57357643635104649</v>
       </c>
       <c r="V45">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W45">
         <f t="shared" si="8"/>
@@ -22268,11 +22514,11 @@
       </c>
       <c r="X45">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y45" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z45" s="41">
         <f t="shared" si="10"/>
@@ -22280,7 +22526,7 @@
       </c>
       <c r="AA45" s="41">
         <f t="shared" si="11"/>
-        <v>-19</v>
+        <v>-21</v>
       </c>
       <c r="AC45">
         <v>3</v>
@@ -22388,19 +22634,19 @@
       </c>
       <c r="S46" s="41">
         <f t="shared" si="30"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="T46" s="41">
         <f t="shared" si="30"/>
-        <v>0.5</v>
+        <v>-0.50000000000000011</v>
       </c>
       <c r="U46" s="41">
         <f t="shared" si="30"/>
-        <v>0.49999999999999978</v>
+        <v>-0.50000000000000044</v>
       </c>
       <c r="V46">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W46">
         <f t="shared" si="8"/>
@@ -22412,7 +22658,7 @@
       </c>
       <c r="Y46" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z46" s="41">
         <f t="shared" si="10"/>
@@ -22510,23 +22756,23 @@
       </c>
       <c r="S47" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="T47" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104605</v>
+        <v>-0.57357643635104616</v>
       </c>
       <c r="U47" s="41">
         <f t="shared" si="30"/>
-        <v>0.42261826174069933</v>
+        <v>-0.42261826174069922</v>
       </c>
       <c r="V47">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W47">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X47">
         <f t="shared" si="9"/>
@@ -22534,11 +22780,11 @@
       </c>
       <c r="Y47" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z47" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA47" s="41">
         <f t="shared" si="11"/>
@@ -22632,23 +22878,23 @@
       </c>
       <c r="S48" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220813</v>
+        <v>0.98480775301220802</v>
       </c>
       <c r="T48" s="41">
         <f t="shared" si="30"/>
-        <v>0.64278760968653914</v>
+        <v>-0.64278760968653925</v>
       </c>
       <c r="U48" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566871</v>
+        <v>-0.3420201433256686</v>
       </c>
       <c r="V48">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W48">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X48">
         <f t="shared" si="9"/>
@@ -22656,11 +22902,11 @@
       </c>
       <c r="Y48" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z48" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA48" s="41">
         <f t="shared" si="11"/>
@@ -22754,23 +23000,23 @@
       </c>
       <c r="S49" s="41">
         <f t="shared" si="30"/>
-        <v>-0.96592582628906842</v>
+        <v>0.96592582628906831</v>
       </c>
       <c r="T49" s="41">
         <f t="shared" si="30"/>
-        <v>0.70710678118654735</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="U49" s="41">
         <f t="shared" si="30"/>
-        <v>0.25881904510252079</v>
+        <v>-0.25881904510252068</v>
       </c>
       <c r="V49">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W49">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X49">
         <f t="shared" si="9"/>
@@ -22778,11 +23024,11 @@
       </c>
       <c r="Y49" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z49" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA49" s="41">
         <f t="shared" si="11"/>
@@ -22875,23 +23121,23 @@
       </c>
       <c r="S50" s="41">
         <f t="shared" si="30"/>
-        <v>-0.93969262078590832</v>
+        <v>0.93969262078590843</v>
       </c>
       <c r="T50" s="41">
         <f t="shared" si="30"/>
-        <v>0.76604444311897779</v>
+        <v>-0.7660444431189779</v>
       </c>
       <c r="U50" s="41">
         <f t="shared" si="30"/>
-        <v>0.1736481776669305</v>
+        <v>-0.17364817766693039</v>
       </c>
       <c r="V50">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W50">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X50">
         <f t="shared" si="9"/>
@@ -22899,11 +23145,11 @@
       </c>
       <c r="Y50" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z50" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA50" s="41">
         <f t="shared" si="11"/>
@@ -22977,23 +23223,23 @@
       </c>
       <c r="S51" s="41">
         <f t="shared" si="30"/>
-        <v>-0.90630778703664994</v>
+        <v>0.90630778703665005</v>
       </c>
       <c r="T51" s="41">
         <f t="shared" si="30"/>
-        <v>0.81915204428899147</v>
+        <v>-0.81915204428899158</v>
       </c>
       <c r="U51" s="41">
         <f t="shared" si="30"/>
-        <v>8.7155742747658443E-2</v>
+        <v>-8.7155742747658319E-2</v>
       </c>
       <c r="V51">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W51">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X51">
         <f t="shared" si="9"/>
@@ -23001,11 +23247,11 @@
       </c>
       <c r="Y51" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z51" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA51" s="41">
         <f t="shared" si="11"/>
@@ -23079,23 +23325,23 @@
       </c>
       <c r="S52" s="41">
         <f t="shared" si="30"/>
-        <v>-0.8660254037844386</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="T52" s="41">
         <f t="shared" si="30"/>
-        <v>0.86602540378443882</v>
+        <v>-0.86602540378443837</v>
       </c>
       <c r="U52" s="41">
         <f t="shared" si="30"/>
-        <v>3.67544536472586E-16</v>
+        <v>-2.45029690981724E-16</v>
       </c>
       <c r="V52">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W52">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X52">
         <f t="shared" si="9"/>
@@ -23103,11 +23349,11 @@
       </c>
       <c r="Y52" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z52" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA52" s="41">
         <f t="shared" si="11"/>
@@ -23181,23 +23427,23 @@
       </c>
       <c r="S53" s="41">
         <f t="shared" si="30"/>
-        <v>-0.8191520442889918</v>
+        <v>0.81915204428899169</v>
       </c>
       <c r="T53" s="41">
         <f t="shared" si="30"/>
-        <v>0.90630778703665005</v>
+        <v>-0.90630778703665005</v>
       </c>
       <c r="U53" s="41">
         <f t="shared" si="30"/>
-        <v>-8.7155742747657708E-2</v>
+        <v>8.7155742747657833E-2</v>
       </c>
       <c r="V53">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W53">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X53">
         <f t="shared" si="9"/>
@@ -23205,11 +23451,11 @@
       </c>
       <c r="Y53" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z53" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA53" s="41">
         <f t="shared" si="11"/>
@@ -23283,23 +23529,23 @@
       </c>
       <c r="S54" s="41">
         <f t="shared" si="30"/>
-        <v>-0.76604444311897812</v>
+        <v>0.76604444311897801</v>
       </c>
       <c r="T54" s="41">
         <f t="shared" si="30"/>
-        <v>0.93969262078590843</v>
+        <v>-0.93969262078590843</v>
       </c>
       <c r="U54" s="41">
         <f t="shared" si="30"/>
-        <v>-0.17364817766692978</v>
+        <v>0.17364817766692991</v>
       </c>
       <c r="V54">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W54">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X54">
         <f t="shared" si="9"/>
@@ -23307,11 +23553,11 @@
       </c>
       <c r="Y54" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z54" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA54" s="41">
         <f t="shared" si="11"/>
@@ -23385,23 +23631,23 @@
       </c>
       <c r="S55" s="41">
         <f t="shared" si="30"/>
-        <v>-0.70710678118654768</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="T55" s="41">
         <f t="shared" si="30"/>
-        <v>0.96592582628906831</v>
+        <v>-0.96592582628906831</v>
       </c>
       <c r="U55" s="41">
         <f t="shared" si="30"/>
-        <v>-0.25881904510252013</v>
+        <v>0.25881904510252024</v>
       </c>
       <c r="V55">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W55">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X55">
         <f t="shared" si="9"/>
@@ -23409,11 +23655,11 @@
       </c>
       <c r="Y55" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z55" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA55" s="41">
         <f t="shared" si="11"/>
@@ -23487,23 +23733,23 @@
       </c>
       <c r="S56" s="41">
         <f t="shared" si="30"/>
-        <v>-0.64278760968653958</v>
+        <v>0.64278760968653947</v>
       </c>
       <c r="T56" s="41">
         <f t="shared" si="30"/>
-        <v>0.98480775301220802</v>
+        <v>-0.98480775301220802</v>
       </c>
       <c r="U56" s="41">
         <f t="shared" si="30"/>
-        <v>-0.34202014332566799</v>
+        <v>0.34202014332566893</v>
       </c>
       <c r="V56">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W56">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X56">
         <f t="shared" si="9"/>
@@ -23511,11 +23757,11 @@
       </c>
       <c r="Y56" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z56" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA56" s="41">
         <f t="shared" si="11"/>
@@ -23589,23 +23835,23 @@
       </c>
       <c r="S57" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104649</v>
+        <v>0.57357643635104594</v>
       </c>
       <c r="T57" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="U57" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069866</v>
+        <v>0.42261826174069955</v>
       </c>
       <c r="V57">
         <f t="shared" si="20"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W57">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X57">
         <f t="shared" si="9"/>
@@ -23613,11 +23859,11 @@
       </c>
       <c r="Y57" s="41">
         <f t="shared" si="21"/>
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="Z57" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA57" s="41">
         <f t="shared" si="11"/>
@@ -23691,15 +23937,15 @@
       </c>
       <c r="S58" s="41">
         <f t="shared" si="30"/>
-        <v>-0.50000000000000044</v>
+        <v>0.49999999999999994</v>
       </c>
       <c r="T58" s="41">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="U58" s="41">
         <f t="shared" si="30"/>
-        <v>-0.49999999999999917</v>
+        <v>0.5</v>
       </c>
       <c r="V58">
         <f t="shared" si="20"/>
@@ -23707,7 +23953,7 @@
       </c>
       <c r="W58">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X58">
         <f t="shared" si="9"/>
@@ -23719,7 +23965,7 @@
       </c>
       <c r="Z58" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA58" s="41">
         <f t="shared" si="11"/>
@@ -23793,15 +24039,15 @@
       </c>
       <c r="S59" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069922</v>
+        <v>0.4226182617406995</v>
       </c>
       <c r="T59" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="U59" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104671</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="V59">
         <f t="shared" si="20"/>
@@ -23809,11 +24055,11 @@
       </c>
       <c r="W59">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X59">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y59" s="41">
         <f t="shared" si="21"/>
@@ -23821,11 +24067,11 @@
       </c>
       <c r="Z59" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA59" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.25">
@@ -23895,15 +24141,15 @@
       </c>
       <c r="S60" s="41">
         <f t="shared" si="30"/>
-        <v>-0.3420201433256686</v>
+        <v>0.34202014332566888</v>
       </c>
       <c r="T60" s="41">
         <f t="shared" si="30"/>
-        <v>0.98480775301220813</v>
+        <v>-0.98480775301220813</v>
       </c>
       <c r="U60" s="41">
         <f t="shared" si="30"/>
-        <v>-0.64278760968653981</v>
+        <v>0.64278760968653914</v>
       </c>
       <c r="V60">
         <f t="shared" si="20"/>
@@ -23911,11 +24157,11 @@
       </c>
       <c r="W60">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X60">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y60" s="41">
         <f t="shared" si="21"/>
@@ -23923,11 +24169,11 @@
       </c>
       <c r="Z60" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA60" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.25">
@@ -23997,15 +24243,15 @@
       </c>
       <c r="S61" s="41">
         <f t="shared" si="30"/>
-        <v>-0.25881904510252068</v>
+        <v>0.25881904510252102</v>
       </c>
       <c r="T61" s="41">
         <f t="shared" si="30"/>
-        <v>0.96592582628906842</v>
+        <v>-0.96592582628906842</v>
       </c>
       <c r="U61" s="41">
         <f t="shared" si="30"/>
-        <v>-0.70710678118654791</v>
+        <v>0.70710678118654735</v>
       </c>
       <c r="V61">
         <f t="shared" si="20"/>
@@ -24013,11 +24259,11 @@
       </c>
       <c r="W61">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X61">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y61" s="41">
         <f t="shared" si="21"/>
@@ -24025,11 +24271,11 @@
       </c>
       <c r="Z61" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA61" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
@@ -24099,15 +24345,15 @@
       </c>
       <c r="S62" s="41">
         <f t="shared" si="30"/>
-        <v>-0.17364817766693039</v>
+        <v>0.17364817766693028</v>
       </c>
       <c r="T62" s="41">
         <f t="shared" si="30"/>
-        <v>0.93969262078590865</v>
+        <v>-0.93969262078590832</v>
       </c>
       <c r="U62" s="41">
         <f t="shared" si="30"/>
-        <v>-0.76604444311897824</v>
+        <v>0.76604444311897779</v>
       </c>
       <c r="V62">
         <f t="shared" si="20"/>
@@ -24115,11 +24361,11 @@
       </c>
       <c r="W62">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X62">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y62" s="41">
         <f t="shared" si="21"/>
@@ -24127,11 +24373,11 @@
       </c>
       <c r="Z62" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA62" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
@@ -24201,15 +24447,15 @@
       </c>
       <c r="S63" s="41">
         <f t="shared" si="30"/>
-        <v>-8.7155742747658319E-2</v>
+        <v>8.7155742747658194E-2</v>
       </c>
       <c r="T63" s="41">
         <f t="shared" si="30"/>
-        <v>0.90630778703665027</v>
+        <v>-0.90630778703664994</v>
       </c>
       <c r="U63" s="41">
         <f t="shared" si="30"/>
-        <v>-0.81915204428899191</v>
+        <v>0.81915204428899147</v>
       </c>
       <c r="V63">
         <f t="shared" si="20"/>
@@ -24217,11 +24463,11 @@
       </c>
       <c r="W63">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X63">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y63" s="41">
         <f t="shared" si="21"/>
@@ -24229,11 +24475,11 @@
       </c>
       <c r="Z63" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA63" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.25">
@@ -24303,15 +24549,15 @@
       </c>
       <c r="S64" s="41">
         <f t="shared" si="30"/>
-        <v>-2.45029690981724E-16</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="T64" s="41">
         <f t="shared" si="30"/>
-        <v>0.86602540378443915</v>
+        <v>-0.8660254037844386</v>
       </c>
       <c r="U64" s="41">
         <f t="shared" si="30"/>
-        <v>-0.86602540378443871</v>
+        <v>0.86602540378443882</v>
       </c>
       <c r="V64">
         <f t="shared" si="20"/>
@@ -24319,11 +24565,11 @@
       </c>
       <c r="W64">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X64">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y64" s="41">
         <f t="shared" si="21"/>
@@ -24331,11 +24577,11 @@
       </c>
       <c r="Z64" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA64" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
@@ -24405,15 +24651,15 @@
       </c>
       <c r="S65" s="41">
         <f t="shared" si="30"/>
-        <v>8.7155742747657833E-2</v>
+        <v>-8.7155742747657944E-2</v>
       </c>
       <c r="T65" s="41">
         <f t="shared" si="30"/>
-        <v>0.81915204428899235</v>
+        <v>-0.8191520442889918</v>
       </c>
       <c r="U65" s="41">
         <f t="shared" si="30"/>
-        <v>-0.90630778703665005</v>
+        <v>0.90630778703665005</v>
       </c>
       <c r="V65">
         <f t="shared" si="20"/>
@@ -24421,11 +24667,11 @@
       </c>
       <c r="W65">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X65">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y65" s="41">
         <f t="shared" si="21"/>
@@ -24433,11 +24679,11 @@
       </c>
       <c r="Z65" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA65" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
@@ -24507,15 +24753,15 @@
       </c>
       <c r="S66" s="41">
         <f t="shared" si="30"/>
-        <v>0.17364817766692991</v>
+        <v>-0.17364817766693047</v>
       </c>
       <c r="T66" s="41">
         <f t="shared" si="30"/>
-        <v>0.76604444311897757</v>
+        <v>-0.76604444311897812</v>
       </c>
       <c r="U66" s="41">
         <f t="shared" si="30"/>
-        <v>-0.93969262078590843</v>
+        <v>0.93969262078590843</v>
       </c>
       <c r="V66">
         <f t="shared" si="20"/>
@@ -24523,11 +24769,11 @@
       </c>
       <c r="W66">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X66">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y66" s="41">
         <f t="shared" si="21"/>
@@ -24535,11 +24781,11 @@
       </c>
       <c r="Z66" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA66" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
@@ -24609,15 +24855,15 @@
       </c>
       <c r="S67" s="41">
         <f t="shared" si="30"/>
-        <v>0.25881904510252024</v>
+        <v>-0.25881904510252079</v>
       </c>
       <c r="T67" s="41">
         <f t="shared" si="30"/>
-        <v>0.70710678118654713</v>
+        <v>-0.70710678118654768</v>
       </c>
       <c r="U67" s="41">
         <f t="shared" si="30"/>
-        <v>-0.9659258262890682</v>
+        <v>0.96592582628906831</v>
       </c>
       <c r="V67">
         <f t="shared" si="20"/>
@@ -24625,11 +24871,11 @@
       </c>
       <c r="W67">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X67">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y67" s="41">
         <f t="shared" si="21"/>
@@ -24637,11 +24883,11 @@
       </c>
       <c r="Z67" s="41">
         <f t="shared" si="10"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA67" s="41">
         <f t="shared" si="11"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
@@ -24711,15 +24957,15 @@
       </c>
       <c r="S68" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566893</v>
+        <v>-0.34202014332566866</v>
       </c>
       <c r="T68" s="41">
         <f t="shared" si="30"/>
-        <v>0.64278760968653903</v>
+        <v>-0.64278760968653958</v>
       </c>
       <c r="U68" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220802</v>
+        <v>0.98480775301220802</v>
       </c>
       <c r="V68">
         <f t="shared" si="20"/>
@@ -24727,11 +24973,11 @@
       </c>
       <c r="W68">
         <f t="shared" ref="W68:W88" si="38">IF(ABS(T68)&gt;0.5,1,0)*SIGN(T68)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X68">
         <f t="shared" ref="X68:X88" si="39">IF(ABS(U68)&gt;0.5,1,0)*SIGN(U68)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y68" s="41">
         <f t="shared" si="21"/>
@@ -24739,11 +24985,11 @@
       </c>
       <c r="Z68" s="41">
         <f t="shared" ref="Z68:Z88" si="40">W68+Z$2</f>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA68" s="41">
         <f t="shared" ref="AA68:AA88" si="41">X68+AA$2</f>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
@@ -24813,15 +25059,15 @@
       </c>
       <c r="S69" s="41">
         <f t="shared" si="30"/>
-        <v>0.42261826174069955</v>
+        <v>-0.42261826174069927</v>
       </c>
       <c r="T69" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104583</v>
+        <v>-0.57357643635104649</v>
       </c>
       <c r="U69" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="V69">
         <f t="shared" ref="V69:V88" si="49">IF(ABS(S69)&gt;0.5,1,0)*SIGN(S69)</f>
@@ -24829,11 +25075,11 @@
       </c>
       <c r="W69">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X69">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y69" s="41">
         <f t="shared" ref="Y69:Y88" si="50">V69+Y$2</f>
@@ -24841,11 +25087,11 @@
       </c>
       <c r="Z69" s="41">
         <f t="shared" si="40"/>
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="AA69" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -24915,15 +25161,15 @@
       </c>
       <c r="S70" s="41">
         <f t="shared" si="30"/>
-        <v>0.5</v>
+        <v>-0.50000000000000011</v>
       </c>
       <c r="T70" s="41">
         <f t="shared" si="30"/>
-        <v>0.49999999999999978</v>
+        <v>-0.50000000000000044</v>
       </c>
       <c r="U70" s="41">
         <f t="shared" si="30"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="V70">
         <f t="shared" si="49"/>
@@ -24935,7 +25181,7 @@
       </c>
       <c r="X70">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y70" s="41">
         <f t="shared" si="50"/>
@@ -24947,7 +25193,7 @@
       </c>
       <c r="AA70" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
@@ -25017,19 +25263,19 @@
       </c>
       <c r="S71" s="41">
         <f t="shared" si="30"/>
-        <v>0.57357643635104605</v>
+        <v>-0.57357643635104616</v>
       </c>
       <c r="T71" s="41">
         <f t="shared" si="30"/>
-        <v>0.42261826174069933</v>
+        <v>-0.42261826174069922</v>
       </c>
       <c r="U71" s="41">
         <f t="shared" si="30"/>
-        <v>-0.99619469809174555</v>
+        <v>0.99619469809174555</v>
       </c>
       <c r="V71">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W71">
         <f t="shared" si="38"/>
@@ -25037,11 +25283,11 @@
       </c>
       <c r="X71">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y71" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z71" s="41">
         <f t="shared" si="40"/>
@@ -25049,7 +25295,7 @@
       </c>
       <c r="AA71" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
@@ -25119,19 +25365,19 @@
       </c>
       <c r="S72" s="41">
         <f t="shared" si="30"/>
-        <v>0.64278760968653914</v>
+        <v>-0.64278760968653925</v>
       </c>
       <c r="T72" s="41">
         <f t="shared" si="30"/>
-        <v>0.34202014332566871</v>
+        <v>-0.3420201433256686</v>
       </c>
       <c r="U72" s="41">
         <f t="shared" si="30"/>
-        <v>-0.98480775301220813</v>
+        <v>0.98480775301220813</v>
       </c>
       <c r="V72">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W72">
         <f t="shared" si="38"/>
@@ -25139,11 +25385,11 @@
       </c>
       <c r="X72">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y72" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z72" s="41">
         <f t="shared" si="40"/>
@@ -25151,7 +25397,7 @@
       </c>
       <c r="AA72" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
@@ -25221,19 +25467,19 @@
       </c>
       <c r="S73" s="41">
         <f t="shared" si="30"/>
-        <v>0.70710678118654735</v>
+        <v>-0.70710678118654746</v>
       </c>
       <c r="T73" s="41">
         <f t="shared" si="30"/>
-        <v>0.25881904510252079</v>
+        <v>-0.25881904510252068</v>
       </c>
       <c r="U73" s="41">
         <f t="shared" si="30"/>
-        <v>-0.96592582628906842</v>
+        <v>0.96592582628906842</v>
       </c>
       <c r="V73">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W73">
         <f t="shared" si="38"/>
@@ -25241,11 +25487,11 @@
       </c>
       <c r="X73">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y73" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z73" s="41">
         <f t="shared" si="40"/>
@@ -25253,7 +25499,7 @@
       </c>
       <c r="AA73" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -25323,19 +25569,19 @@
       </c>
       <c r="S74" s="41">
         <f t="shared" si="30"/>
-        <v>0.76604444311897779</v>
+        <v>-0.7660444431189779</v>
       </c>
       <c r="T74" s="41">
         <f t="shared" si="30"/>
-        <v>0.1736481776669305</v>
+        <v>-0.17364817766693039</v>
       </c>
       <c r="U74" s="41">
         <f t="shared" si="30"/>
-        <v>-0.93969262078590865</v>
+        <v>0.93969262078590865</v>
       </c>
       <c r="V74">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W74">
         <f t="shared" si="38"/>
@@ -25343,11 +25589,11 @@
       </c>
       <c r="X74">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y74" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z74" s="41">
         <f t="shared" si="40"/>
@@ -25355,7 +25601,7 @@
       </c>
       <c r="AA74" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
@@ -25425,19 +25671,19 @@
       </c>
       <c r="S75" s="41">
         <f t="shared" si="30"/>
-        <v>0.81915204428899147</v>
+        <v>-0.81915204428899158</v>
       </c>
       <c r="T75" s="41">
         <f t="shared" si="30"/>
-        <v>8.7155742747658443E-2</v>
+        <v>-8.7155742747658319E-2</v>
       </c>
       <c r="U75" s="41">
         <f t="shared" si="30"/>
-        <v>-0.90630778703665038</v>
+        <v>0.90630778703665027</v>
       </c>
       <c r="V75">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W75">
         <f t="shared" si="38"/>
@@ -25445,11 +25691,11 @@
       </c>
       <c r="X75">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y75" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z75" s="41">
         <f t="shared" si="40"/>
@@ -25457,7 +25703,7 @@
       </c>
       <c r="AA75" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
@@ -25527,19 +25773,19 @@
       </c>
       <c r="S76" s="41">
         <f t="shared" si="30"/>
-        <v>0.86602540378443882</v>
+        <v>-0.86602540378443837</v>
       </c>
       <c r="T76" s="41">
         <f t="shared" si="30"/>
-        <v>3.67544536472586E-16</v>
+        <v>-2.45029690981724E-16</v>
       </c>
       <c r="U76" s="41">
         <f t="shared" si="30"/>
-        <v>-0.86602540378443915</v>
+        <v>0.86602540378443915</v>
       </c>
       <c r="V76">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W76">
         <f t="shared" si="38"/>
@@ -25547,11 +25793,11 @@
       </c>
       <c r="X76">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y76" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z76" s="41">
         <f t="shared" si="40"/>
@@ -25559,7 +25805,7 @@
       </c>
       <c r="AA76" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
@@ -25629,19 +25875,19 @@
       </c>
       <c r="S77" s="41">
         <f t="shared" si="30"/>
-        <v>0.90630778703665005</v>
+        <v>-0.90630778703665005</v>
       </c>
       <c r="T77" s="41">
         <f t="shared" si="30"/>
-        <v>-8.7155742747657708E-2</v>
+        <v>8.7155742747657833E-2</v>
       </c>
       <c r="U77" s="41">
         <f t="shared" si="30"/>
-        <v>-0.81915204428899147</v>
+        <v>0.81915204428899235</v>
       </c>
       <c r="V77">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W77">
         <f t="shared" si="38"/>
@@ -25649,11 +25895,11 @@
       </c>
       <c r="X77">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y77" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z77" s="41">
         <f t="shared" si="40"/>
@@ -25661,7 +25907,7 @@
       </c>
       <c r="AA77" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -25731,19 +25977,19 @@
       </c>
       <c r="S78" s="41">
         <f t="shared" si="30"/>
-        <v>0.93969262078590843</v>
+        <v>-0.93969262078590843</v>
       </c>
       <c r="T78" s="41">
         <f t="shared" si="30"/>
-        <v>-0.17364817766692978</v>
+        <v>0.17364817766692991</v>
       </c>
       <c r="U78" s="41">
         <f t="shared" si="30"/>
-        <v>-0.76604444311897768</v>
+        <v>0.76604444311897757</v>
       </c>
       <c r="V78">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W78">
         <f t="shared" si="38"/>
@@ -25751,11 +25997,11 @@
       </c>
       <c r="X78">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y78" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z78" s="41">
         <f t="shared" si="40"/>
@@ -25763,7 +26009,7 @@
       </c>
       <c r="AA78" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
@@ -25833,19 +26079,19 @@
       </c>
       <c r="S79" s="41">
         <f t="shared" si="30"/>
-        <v>0.96592582628906831</v>
+        <v>-0.96592582628906831</v>
       </c>
       <c r="T79" s="41">
         <f t="shared" si="30"/>
-        <v>-0.25881904510252013</v>
+        <v>0.25881904510252024</v>
       </c>
       <c r="U79" s="41">
         <f t="shared" si="30"/>
-        <v>-0.70710678118654724</v>
+        <v>0.70710678118654713</v>
       </c>
       <c r="V79">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W79">
         <f t="shared" si="38"/>
@@ -25853,11 +26099,11 @@
       </c>
       <c r="X79">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y79" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z79" s="41">
         <f t="shared" si="40"/>
@@ -25865,7 +26111,7 @@
       </c>
       <c r="AA79" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
@@ -25935,19 +26181,19 @@
       </c>
       <c r="S80" s="41">
         <f t="shared" si="30"/>
-        <v>0.98480775301220802</v>
+        <v>-0.98480775301220802</v>
       </c>
       <c r="T80" s="41">
         <f t="shared" si="30"/>
-        <v>-0.34202014332566799</v>
+        <v>0.34202014332566893</v>
       </c>
       <c r="U80" s="41">
         <f t="shared" si="30"/>
-        <v>-0.64278760968653903</v>
+        <v>0.64278760968653903</v>
       </c>
       <c r="V80">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W80">
         <f t="shared" si="38"/>
@@ -25955,11 +26201,11 @@
       </c>
       <c r="X80">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y80" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z80" s="41">
         <f t="shared" si="40"/>
@@ -25967,7 +26213,7 @@
       </c>
       <c r="AA80" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
@@ -26037,19 +26283,19 @@
       </c>
       <c r="S81" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="T81" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069866</v>
+        <v>0.42261826174069955</v>
       </c>
       <c r="U81" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104594</v>
+        <v>0.57357643635104583</v>
       </c>
       <c r="V81">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W81">
         <f t="shared" si="38"/>
@@ -26057,11 +26303,11 @@
       </c>
       <c r="X81">
         <f t="shared" si="39"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y81" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z81" s="41">
         <f t="shared" si="40"/>
@@ -26069,7 +26315,7 @@
       </c>
       <c r="AA81" s="41">
         <f t="shared" si="41"/>
-        <v>-21</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -26139,19 +26385,19 @@
       </c>
       <c r="S82" s="41">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T82" s="41">
         <f t="shared" si="30"/>
-        <v>-0.49999999999999917</v>
+        <v>0.5</v>
       </c>
       <c r="U82" s="41">
         <f t="shared" si="30"/>
-        <v>-0.49999999999999989</v>
+        <v>0.49999999999999978</v>
       </c>
       <c r="V82">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W82">
         <f t="shared" si="38"/>
@@ -26163,7 +26409,7 @@
       </c>
       <c r="Y82" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z82" s="41">
         <f t="shared" si="40"/>
@@ -26241,23 +26487,23 @@
       </c>
       <c r="S83" s="41">
         <f t="shared" si="30"/>
-        <v>0.99619469809174555</v>
+        <v>-0.99619469809174555</v>
       </c>
       <c r="T83" s="41">
         <f t="shared" si="30"/>
-        <v>-0.57357643635104671</v>
+        <v>0.57357643635104605</v>
       </c>
       <c r="U83" s="41">
         <f t="shared" si="30"/>
-        <v>-0.42261826174069944</v>
+        <v>0.42261826174069933</v>
       </c>
       <c r="V83">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W83">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X83">
         <f t="shared" si="39"/>
@@ -26265,11 +26511,11 @@
       </c>
       <c r="Y83" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z83" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA83" s="41">
         <f t="shared" si="41"/>
@@ -26343,23 +26589,23 @@
       </c>
       <c r="S84" s="41">
         <f t="shared" ref="S84:U88" si="54">SIN( ($A84+S$2)*deg2rad)</f>
-        <v>0.98480775301220813</v>
+        <v>-0.98480775301220813</v>
       </c>
       <c r="T84" s="41">
         <f t="shared" si="54"/>
-        <v>-0.64278760968653981</v>
+        <v>0.64278760968653914</v>
       </c>
       <c r="U84" s="41">
         <f t="shared" si="54"/>
-        <v>-0.34202014332566882</v>
+        <v>0.34202014332566871</v>
       </c>
       <c r="V84">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W84">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X84">
         <f t="shared" si="39"/>
@@ -26367,11 +26613,11 @@
       </c>
       <c r="Y84" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z84" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA84" s="41">
         <f t="shared" si="41"/>
@@ -26445,23 +26691,23 @@
       </c>
       <c r="S85" s="41">
         <f t="shared" si="54"/>
-        <v>0.96592582628906842</v>
+        <v>-0.96592582628906842</v>
       </c>
       <c r="T85" s="41">
         <f t="shared" si="54"/>
-        <v>-0.70710678118654791</v>
+        <v>0.70710678118654735</v>
       </c>
       <c r="U85" s="41">
         <f t="shared" si="54"/>
-        <v>-0.25881904510252096</v>
+        <v>0.25881904510252079</v>
       </c>
       <c r="V85">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W85">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X85">
         <f t="shared" si="39"/>
@@ -26469,11 +26715,11 @@
       </c>
       <c r="Y85" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z85" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA85" s="41">
         <f t="shared" si="41"/>
@@ -26547,23 +26793,23 @@
       </c>
       <c r="S86" s="41">
         <f t="shared" si="54"/>
-        <v>0.93969262078590865</v>
+        <v>-0.93969262078590832</v>
       </c>
       <c r="T86" s="41">
         <f t="shared" si="54"/>
-        <v>-0.76604444311897824</v>
+        <v>0.76604444311897779</v>
       </c>
       <c r="U86" s="41">
         <f t="shared" si="54"/>
-        <v>-0.17364817766693064</v>
+        <v>0.1736481776669305</v>
       </c>
       <c r="V86">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W86">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X86">
         <f t="shared" si="39"/>
@@ -26571,11 +26817,11 @@
       </c>
       <c r="Y86" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z86" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA86" s="41">
         <f t="shared" si="41"/>
@@ -26649,23 +26895,23 @@
       </c>
       <c r="S87" s="41">
         <f t="shared" si="54"/>
-        <v>0.90630778703665027</v>
+        <v>-0.90630778703664994</v>
       </c>
       <c r="T87" s="41">
         <f t="shared" si="54"/>
-        <v>-0.81915204428899191</v>
+        <v>0.81915204428899147</v>
       </c>
       <c r="U87" s="41">
         <f t="shared" si="54"/>
-        <v>-8.7155742747658554E-2</v>
+        <v>8.7155742747658443E-2</v>
       </c>
       <c r="V87">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W87">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X87">
         <f t="shared" si="39"/>
@@ -26673,11 +26919,11 @@
       </c>
       <c r="Y87" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z87" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA87" s="41">
         <f t="shared" si="41"/>
@@ -26751,23 +26997,23 @@
       </c>
       <c r="S88" s="41">
         <f t="shared" si="54"/>
-        <v>0.86602540378443915</v>
+        <v>-0.8660254037844386</v>
       </c>
       <c r="T88" s="41">
         <f t="shared" si="54"/>
-        <v>-0.86602540378443871</v>
+        <v>0.86602540378443882</v>
       </c>
       <c r="U88" s="41">
         <f t="shared" si="54"/>
-        <v>-4.90059381963448E-16</v>
+        <v>3.67544536472586E-16</v>
       </c>
       <c r="V88">
         <f t="shared" si="49"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W88">
         <f t="shared" si="38"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X88">
         <f t="shared" si="39"/>
@@ -26775,11 +27021,11 @@
       </c>
       <c r="Y88" s="41">
         <f t="shared" si="50"/>
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="Z88" s="41">
         <f t="shared" si="40"/>
-        <v>-18</v>
+        <v>-16</v>
       </c>
       <c r="AA88" s="41">
         <f t="shared" si="41"/>
@@ -26792,7 +27038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D0068D-F33F-44A4-9DEF-2D0781A661B6}">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -27095,7 +27341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BAE66D-154B-4C32-935A-061D0922E860}">
   <dimension ref="A1:I52"/>
   <sheetViews>
@@ -27878,18 +28124,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29800C5-F2DC-491C-A496-777CBE6FE60C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Sin tes and trying to get melexis working.
</commit_message>
<xml_diff>
--- a/Pins for HoverBoard wheel.xlsx
+++ b/Pins for HoverBoard wheel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,12 +23,10 @@
     <sheet name="sin Pulse syntesis" sheetId="12" r:id="rId9"/>
     <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <definedNames>
     <definedName name="amplitude">'sin Pulse syntesis'!$H$2</definedName>
     <definedName name="deg2rad">'3 Hall Synthesis'!$B$1</definedName>
+    <definedName name="Eta">'sin Pulse syntesis'!$H$5</definedName>
     <definedName name="frequency">'sin Pulse syntesis'!$H$1</definedName>
     <definedName name="omega">'sin Pulse syntesis'!$H$3</definedName>
     <definedName name="omegaTerm">'sin Pulse syntesis'!$H$4</definedName>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="295">
   <si>
     <t>Pin out</t>
   </si>
@@ -938,6 +936,18 @@
   </si>
   <si>
     <t>gnd</t>
+  </si>
+  <si>
+    <t>Eta</t>
+  </si>
+  <si>
+    <t>damped</t>
+  </si>
+  <si>
+    <t>Ribbon 9</t>
+  </si>
+  <si>
+    <t>Saleae</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1041,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1352,12 +1362,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1566,6 +1585,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7592,18 +7615,20 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet1!$C$1</c:f>
+              <c:f>'sin Pulse syntesis'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>output</c:v>
+                  <c:v>damped</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -7625,7 +7650,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$B$2:$B$52</c:f>
+              <c:f>'sin Pulse syntesis'!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -7633,161 +7658,161 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.04</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.44</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.48</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.52</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.6</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.64</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.68</c:v>
+                  <c:v>1.02</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.72</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.76</c:v>
+                  <c:v>1.1399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.8</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.84</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.88</c:v>
+                  <c:v>1.32</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.92</c:v>
+                  <c:v>1.38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.96</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.04</c:v>
+                  <c:v>1.56</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.08</c:v>
+                  <c:v>1.62</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>1.68</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1599999999999999</c:v>
+                  <c:v>1.74</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.2</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.24</c:v>
+                  <c:v>1.86</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.28</c:v>
+                  <c:v>1.92</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.32</c:v>
+                  <c:v>1.98</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.36</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.4</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.44</c:v>
+                  <c:v>2.16</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.48</c:v>
+                  <c:v>2.2200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.52</c:v>
+                  <c:v>2.2799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.56</c:v>
+                  <c:v>2.34</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.6</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.64</c:v>
+                  <c:v>2.46</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.68</c:v>
+                  <c:v>2.52</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.72</c:v>
+                  <c:v>2.58</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.76</c:v>
+                  <c:v>2.64</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.8</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.84</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.88</c:v>
+                  <c:v>2.82</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.92</c:v>
+                  <c:v>2.88</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.96</c:v>
+                  <c:v>2.94</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$C$2:$C$52</c:f>
+              <c:f>'sin Pulse syntesis'!$D$2:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -7795,154 +7820,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.959974558897578</c:v>
+                  <c:v>194.28539565415954</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.415921227037956</c:v>
+                  <c:v>215.095422497675</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.871760934592871</c:v>
+                  <c:v>65.818736006415762</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122.84718689593738</c:v>
+                  <c:v>-117.90390522320961</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149.88523933458066</c:v>
+                  <c:v>-188.90864627383806</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>174.5595120118156</c:v>
+                  <c:v>-104.57138311122746</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>196.48087690782626</c:v>
+                  <c:v>51.774851522830915</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>215.3036210030138</c:v>
+                  <c:v>150.06698412287409</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230.73089837883498</c:v>
+                  <c:v>120.22057610127892</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>242.51941165526415</c:v>
+                  <c:v>5.1436743191729821E-14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>250.4832489358156</c:v>
+                  <c:v>-106.62608585813452</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>254.49681574920925</c:v>
+                  <c:v>-118.04687073728491</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>254.49681574920925</c:v>
+                  <c:v>-36.122088193321886</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>250.48324893581562</c:v>
+                  <c:v>64.70703512742466</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>242.51941165526418</c:v>
+                  <c:v>103.67526323385277</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>230.73089837883501</c:v>
+                  <c:v>57.38999185388802</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>215.30362100301386</c:v>
+                  <c:v>-28.414640972770254</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>196.48087690782626</c:v>
+                  <c:v>-82.358507080170796</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>174.55951201181566</c:v>
+                  <c:v>-65.978451062309219</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>149.88523933458069</c:v>
+                  <c:v>-5.645816637280305E-14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>122.84718689593748</c:v>
+                  <c:v>58.517636630105002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>93.871760934592928</c:v>
+                  <c:v>64.785496265109373</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63.415921227037977</c:v>
+                  <c:v>19.824222320509609</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31.959974558897656</c:v>
+                  <c:v>-35.51197381507555</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.124128560016981E-14</c:v>
+                  <c:v>-56.898190837849604</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-31.959974558897478</c:v>
+                  <c:v>-31.496295324755145</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-63.415921227037913</c:v>
+                  <c:v>15.594285601290384</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-93.871760934592871</c:v>
+                  <c:v>45.199307016929993</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-122.84718689593733</c:v>
+                  <c:v>36.209741674455593</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-149.88523933458063</c:v>
+                  <c:v>4.6477347986890172E-14</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-174.55951201181554</c:v>
+                  <c:v>-32.115159899323643</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-196.48087690782614</c:v>
+                  <c:v>-35.555034200418127</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-215.30362100301377</c:v>
+                  <c:v>-10.879763886010611</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-230.73089837883492</c:v>
+                  <c:v>19.489384450379923</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-242.51941165526415</c:v>
+                  <c:v>31.226389204510387</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-250.48324893581562</c:v>
+                  <c:v>17.285533368079516</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-254.49681574920925</c:v>
+                  <c:v>-8.558325394561777</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-254.49681574920925</c:v>
+                  <c:v>-24.805905634277575</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-250.48324893581562</c:v>
+                  <c:v>-19.872327570900037</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-242.51941165526418</c:v>
+                  <c:v>-3.4009745853328808E-14</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-230.73089837883498</c:v>
+                  <c:v>17.625173447769122</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-215.30362100301394</c:v>
+                  <c:v>19.513016490910516</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-196.48087690782634</c:v>
+                  <c:v>5.9709410185981922</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-174.55951201181568</c:v>
+                  <c:v>-10.696000966678424</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-149.88523933458072</c:v>
+                  <c:v>-17.137405748636187</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-122.84718689593741</c:v>
+                  <c:v>-9.4865018484935622</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-93.87176093459307</c:v>
+                  <c:v>4.696908562014448</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-63.415921227038112</c:v>
+                  <c:v>13.613769655941891</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-31.959974558897684</c:v>
+                  <c:v>10.906164607182053</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-6.2482571200339621E-14</c:v>
+                  <c:v>-2.1773015367426657E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7950,7 +7975,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D5A2-4FB3-A6EE-7A55A7B8821C}"/>
+              <c16:uniqueId val="{00000000-EC5C-44D5-BC83-BB8393E66A4E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7962,11 +7987,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109187887"/>
-        <c:axId val="2107002143"/>
+        <c:axId val="586436703"/>
+        <c:axId val="587490159"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109187887"/>
+        <c:axId val="586436703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8023,12 +8048,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107002143"/>
+        <c:crossAx val="587490159"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2107002143"/>
+        <c:axId val="587490159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8085,7 +8110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109187887"/>
+        <c:crossAx val="586436703"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10670,28 +10695,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E549A80-CF78-4895-B266-22E77AF00ACA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BA57615-3784-402F-9C76-494B9AC89C6F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -10706,433 +10729,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>output</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>0</v>
-          </cell>
-          <cell r="C2">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.04</v>
-          </cell>
-          <cell r="C3">
-            <v>31.959974558897578</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>0.08</v>
-          </cell>
-          <cell r="C4">
-            <v>63.415921227037956</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>0.12</v>
-          </cell>
-          <cell r="C5">
-            <v>93.871760934592871</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>0.16</v>
-          </cell>
-          <cell r="C6">
-            <v>122.84718689593738</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>0.2</v>
-          </cell>
-          <cell r="C7">
-            <v>149.88523933458066</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>0.24</v>
-          </cell>
-          <cell r="C8">
-            <v>174.5595120118156</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>0.28000000000000003</v>
-          </cell>
-          <cell r="C9">
-            <v>196.48087690782626</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>0.32</v>
-          </cell>
-          <cell r="C10">
-            <v>215.3036210030138</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>0.36</v>
-          </cell>
-          <cell r="C11">
-            <v>230.73089837883498</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>0.4</v>
-          </cell>
-          <cell r="C12">
-            <v>242.51941165526415</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>0.44</v>
-          </cell>
-          <cell r="C13">
-            <v>250.4832489358156</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>0.48</v>
-          </cell>
-          <cell r="C14">
-            <v>254.49681574920925</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>0.52</v>
-          </cell>
-          <cell r="C15">
-            <v>254.49681574920925</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>0.56000000000000005</v>
-          </cell>
-          <cell r="C16">
-            <v>250.48324893581562</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>0.6</v>
-          </cell>
-          <cell r="C17">
-            <v>242.51941165526418</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>0.64</v>
-          </cell>
-          <cell r="C18">
-            <v>230.73089837883501</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>0.68</v>
-          </cell>
-          <cell r="C19">
-            <v>215.30362100301386</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>0.72</v>
-          </cell>
-          <cell r="C20">
-            <v>196.48087690782626</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>0.76</v>
-          </cell>
-          <cell r="C21">
-            <v>174.55951201181566</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>0.8</v>
-          </cell>
-          <cell r="C22">
-            <v>149.88523933458069</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>0.84</v>
-          </cell>
-          <cell r="C23">
-            <v>122.84718689593748</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>0.88</v>
-          </cell>
-          <cell r="C24">
-            <v>93.871760934592928</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>0.92</v>
-          </cell>
-          <cell r="C25">
-            <v>63.415921227037977</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>0.96</v>
-          </cell>
-          <cell r="C26">
-            <v>31.959974558897656</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>1</v>
-          </cell>
-          <cell r="C27">
-            <v>3.124128560016981E-14</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>1.04</v>
-          </cell>
-          <cell r="C28">
-            <v>-31.959974558897478</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>1.08</v>
-          </cell>
-          <cell r="C29">
-            <v>-63.415921227037913</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>1.1200000000000001</v>
-          </cell>
-          <cell r="C30">
-            <v>-93.871760934592871</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>1.1599999999999999</v>
-          </cell>
-          <cell r="C31">
-            <v>-122.84718689593733</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32">
-            <v>1.2</v>
-          </cell>
-          <cell r="C32">
-            <v>-149.88523933458063</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="B33">
-            <v>1.24</v>
-          </cell>
-          <cell r="C33">
-            <v>-174.55951201181554</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34">
-            <v>1.28</v>
-          </cell>
-          <cell r="C34">
-            <v>-196.48087690782614</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35">
-            <v>1.32</v>
-          </cell>
-          <cell r="C35">
-            <v>-215.30362100301377</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36">
-            <v>1.36</v>
-          </cell>
-          <cell r="C36">
-            <v>-230.73089837883492</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37">
-            <v>1.4</v>
-          </cell>
-          <cell r="C37">
-            <v>-242.51941165526415</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38">
-            <v>1.44</v>
-          </cell>
-          <cell r="C38">
-            <v>-250.48324893581562</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="B39">
-            <v>1.48</v>
-          </cell>
-          <cell r="C39">
-            <v>-254.49681574920925</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="B40">
-            <v>1.52</v>
-          </cell>
-          <cell r="C40">
-            <v>-254.49681574920925</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41">
-            <v>1.56</v>
-          </cell>
-          <cell r="C41">
-            <v>-250.48324893581562</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42">
-            <v>1.6</v>
-          </cell>
-          <cell r="C42">
-            <v>-242.51941165526418</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43">
-            <v>1.64</v>
-          </cell>
-          <cell r="C43">
-            <v>-230.73089837883498</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44">
-            <v>1.68</v>
-          </cell>
-          <cell r="C44">
-            <v>-215.30362100301394</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="B45">
-            <v>1.72</v>
-          </cell>
-          <cell r="C45">
-            <v>-196.48087690782634</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="B46">
-            <v>1.76</v>
-          </cell>
-          <cell r="C46">
-            <v>-174.55951201181568</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47">
-            <v>1.8</v>
-          </cell>
-          <cell r="C47">
-            <v>-149.88523933458072</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48">
-            <v>1.84</v>
-          </cell>
-          <cell r="C48">
-            <v>-122.84718689593741</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49">
-            <v>1.88</v>
-          </cell>
-          <cell r="C49">
-            <v>-93.87176093459307</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50">
-            <v>1.92</v>
-          </cell>
-          <cell r="C50">
-            <v>-63.415921227038112</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51">
-            <v>1.96</v>
-          </cell>
-          <cell r="C51">
-            <v>-31.959974558897684</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52">
-            <v>2</v>
-          </cell>
-          <cell r="C52">
-            <v>-6.2482571200339621E-14</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11929,10 +11525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B464C57-0DBE-40E5-955E-B8EBE134B27C}">
-  <dimension ref="A1:Y63"/>
+  <dimension ref="A1:AB63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M80" sqref="M80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11940,7 +11536,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="62"/>
       <c r="B1" s="63" t="s">
         <v>155</v>
@@ -11980,8 +11576,14 @@
         <v>157</v>
       </c>
       <c r="W1" s="49"/>
-    </row>
-    <row r="2" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA1" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="66" t="s">
         <v>233</v>
       </c>
@@ -12045,8 +11647,11 @@
       <c r="Y2" s="61" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA2" s="93" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>162</v>
       </c>
@@ -12100,7 +11705,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>162</v>
       </c>
@@ -12153,8 +11758,14 @@
       <c r="V4" s="53" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA4">
+        <v>6</v>
+      </c>
+      <c r="AB4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>162</v>
       </c>
@@ -12207,8 +11818,14 @@
       <c r="W5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA5">
+        <v>7</v>
+      </c>
+      <c r="AB5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>162</v>
       </c>
@@ -12263,8 +11880,14 @@
         <v>4</v>
       </c>
       <c r="X6" s="49"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>162</v>
       </c>
@@ -12317,8 +11940,14 @@
       <c r="W7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>8</v>
+      </c>
+      <c r="AB7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>162</v>
       </c>
@@ -12371,8 +12000,14 @@
       <c r="W8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66"/>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
@@ -12415,7 +12050,7 @@
       </c>
       <c r="W9" s="58"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>186</v>
       </c>
@@ -12470,8 +12105,14 @@
       <c r="Y10" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA10">
+        <v>3</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>186</v>
       </c>
@@ -12522,7 +12163,7 @@
       </c>
       <c r="W11" s="58"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>186</v>
       </c>
@@ -12577,8 +12218,14 @@
       <c r="Y12" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA12">
+        <v>4</v>
+      </c>
+      <c r="AB12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>186</v>
       </c>
@@ -12630,7 +12277,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="66"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
@@ -12677,8 +12324,14 @@
       <c r="Y14" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA14">
+        <v>5</v>
+      </c>
+      <c r="AB14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="66" t="s">
         <v>144</v>
       </c>
@@ -12733,7 +12386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
         <v>144</v>
       </c>
@@ -12788,7 +12441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
         <v>144</v>
       </c>
@@ -12845,7 +12498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="66" t="s">
         <v>144</v>
       </c>
@@ -12902,7 +12555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="66" t="s">
         <v>144</v>
       </c>
@@ -12957,7 +12610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="66"/>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -13002,7 +12655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="66" t="s">
         <v>210</v>
       </c>
@@ -13042,7 +12695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="68" t="s">
         <v>210</v>
       </c>
@@ -13084,8 +12737,14 @@
       <c r="X22">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="AA22">
+        <v>9</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>150</v>
       </c>
@@ -13099,7 +12758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1</v>
       </c>
@@ -13116,7 +12775,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -13133,7 +12792,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -13150,7 +12809,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>4</v>
       </c>
@@ -13167,7 +12826,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>5</v>
       </c>
@@ -13184,7 +12843,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>6</v>
       </c>
@@ -13199,7 +12858,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>7</v>
       </c>
@@ -13216,7 +12875,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>8</v>
       </c>
@@ -27343,18 +27002,19 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BAE66D-154B-4C32-935A-061D0922E860}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>272</v>
       </c>
@@ -27364,17 +27024,24 @@
       <c r="C1" t="s">
         <v>274</v>
       </c>
+      <c r="D1" t="s">
+        <v>292</v>
+      </c>
       <c r="G1" t="s">
         <v>275</v>
       </c>
       <c r="H1">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="I1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O1">
+        <f>30/12</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -27383,7 +27050,11 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C33" si="0">amplitude*SIN(A2  /omegaTerm)</f>
+        <f>amplitude*SIN(A2  /omegaTerm)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D33" si="0">EXP(Eta*A2)*C2</f>
         <v>0</v>
       </c>
       <c r="G2" t="s">
@@ -27396,728 +27067,939 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A52" si="1">A2+$H$6</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B52" si="2">A3/1000</f>
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C33" si="3">amplitude*SIN(A3  /omegaTerm)</f>
+        <v>206.29933356561159</v>
+      </c>
+      <c r="D3">
         <f t="shared" si="0"/>
-        <v>31.959974558897578</v>
+        <v>194.28539565415954</v>
       </c>
       <c r="G3" t="s">
         <v>279</v>
       </c>
       <c r="H3">
         <f>2*PI()*frequency</f>
-        <v>3.1415926535897931</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15.707963267948966</v>
+      </c>
+      <c r="O3" s="92">
+        <f>30/12</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="C4">
+        <f t="shared" si="3"/>
+        <v>242.51941165526418</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>63.415921227037956</v>
+        <v>215.095422497675</v>
       </c>
       <c r="G4" t="s">
         <v>280</v>
       </c>
       <c r="H4">
         <f>1000/omega</f>
-        <v>318.3098861837907</v>
+        <v>63.661977236758133</v>
       </c>
       <c r="I4">
         <f>1000 / (2*PI()*frequency)</f>
-        <v>318.3098861837907</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63.661977236758133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f t="shared" si="2"/>
-        <v>0.12</v>
+        <v>0.18</v>
       </c>
       <c r="C5">
+        <f t="shared" si="3"/>
+        <v>78.799333565611619</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>93.871760934592871</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65.818736006415762</v>
+      </c>
+      <c r="G5" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5">
+        <f>-1/1000</f>
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="B6">
         <f t="shared" si="2"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="C6">
+        <f t="shared" si="3"/>
+        <v>-149.88523933458063</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>122.84718689593738</v>
+        <v>-117.90390522320961</v>
       </c>
       <c r="G6" t="s">
         <v>281</v>
       </c>
       <c r="H6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="B7">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C7">
+        <f t="shared" si="3"/>
+        <v>-255</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>149.88523933458066</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-188.90864627383806</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B8">
         <f t="shared" si="2"/>
-        <v>0.24</v>
+        <v>0.36</v>
       </c>
       <c r="C8">
+        <f t="shared" si="3"/>
+        <v>-149.88523933458072</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>174.5595120118156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-104.57138311122746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="B9">
         <f t="shared" si="2"/>
-        <v>0.28000000000000003</v>
+        <v>0.42</v>
       </c>
       <c r="C9">
+        <f t="shared" si="3"/>
+        <v>78.799333565611533</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>196.48087690782626</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51.774851522830915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>480</v>
       </c>
       <c r="B10">
         <f t="shared" si="2"/>
-        <v>0.32</v>
+        <v>0.48</v>
       </c>
       <c r="C10">
+        <f t="shared" si="3"/>
+        <v>242.51941165526415</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>215.3036210030138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150.06698412287409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
-        <v>360</v>
+        <v>540</v>
       </c>
       <c r="B11">
         <f t="shared" si="2"/>
-        <v>0.36</v>
+        <v>0.54</v>
       </c>
       <c r="C11">
+        <f t="shared" si="3"/>
+        <v>206.29933356561165</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>230.73089837883498</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120.22057610127892</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="B12">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C12">
+        <f t="shared" si="3"/>
+        <v>9.3723856800509431E-14</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
-        <v>242.51941165526415</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.1436743191729821E-14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
-        <v>440</v>
+        <v>660</v>
       </c>
       <c r="B13">
         <f t="shared" si="2"/>
-        <v>0.44</v>
+        <v>0.66</v>
       </c>
       <c r="C13">
+        <f t="shared" si="3"/>
+        <v>-206.29933356561153</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
-        <v>250.4832489358156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-106.62608585813452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="B14">
         <f t="shared" si="2"/>
-        <v>0.48</v>
+        <v>0.72</v>
       </c>
       <c r="C14">
+        <f t="shared" si="3"/>
+        <v>-242.51941165526421</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
-        <v>254.49681574920925</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-118.04687073728491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>780</v>
       </c>
       <c r="B15">
         <f t="shared" si="2"/>
-        <v>0.52</v>
+        <v>0.78</v>
       </c>
       <c r="C15">
+        <f t="shared" si="3"/>
+        <v>-78.799333565611718</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
-        <v>254.49681574920925</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-36.122088193321886</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
-        <v>560</v>
+        <v>840</v>
       </c>
       <c r="B16">
         <f t="shared" si="2"/>
-        <v>0.56000000000000005</v>
+        <v>0.84</v>
       </c>
       <c r="C16">
+        <f t="shared" si="3"/>
+        <v>149.88523933458055</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
-        <v>250.48324893581562</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64.70703512742466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="B17">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="C17">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>242.51941165526418</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103.67526323385277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
-        <v>640</v>
+        <v>960</v>
       </c>
       <c r="B18">
         <f t="shared" si="2"/>
-        <v>0.64</v>
+        <v>0.96</v>
       </c>
       <c r="C18">
+        <f t="shared" si="3"/>
+        <v>149.88523933458077</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
-        <v>230.73089837883501</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57.38999185388802</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
-        <v>680</v>
+        <v>1020</v>
       </c>
       <c r="B19">
         <f t="shared" si="2"/>
-        <v>0.68</v>
+        <v>1.02</v>
       </c>
       <c r="C19">
+        <f t="shared" si="3"/>
+        <v>-78.799333565611875</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
-        <v>215.30362100301386</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-28.414640972770254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="B20">
         <f t="shared" si="2"/>
-        <v>0.72</v>
+        <v>1.08</v>
       </c>
       <c r="C20">
+        <f t="shared" si="3"/>
+        <v>-242.51941165526412</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="0"/>
-        <v>196.48087690782626</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-82.358507080170796</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
-        <v>760</v>
+        <v>1140</v>
       </c>
       <c r="B21">
         <f t="shared" si="2"/>
-        <v>0.76</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C21">
+        <f t="shared" si="3"/>
+        <v>-206.29933356561142</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="0"/>
-        <v>174.55951201181566</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-65.978451062309219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="B22">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="C22">
+        <f t="shared" si="3"/>
+        <v>-1.8744771360101886E-13</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="0"/>
-        <v>149.88523933458069</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-5.645816637280305E-14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
-        <v>840</v>
+        <v>1260</v>
       </c>
       <c r="B23">
         <f t="shared" si="2"/>
-        <v>0.84</v>
+        <v>1.26</v>
       </c>
       <c r="C23">
+        <f t="shared" si="3"/>
+        <v>206.29933356561173</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="0"/>
-        <v>122.84718689593748</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58.517636630105002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
-        <v>880</v>
+        <v>1320</v>
       </c>
       <c r="B24">
         <f t="shared" si="2"/>
-        <v>0.88</v>
+        <v>1.32</v>
       </c>
       <c r="C24">
+        <f t="shared" si="3"/>
+        <v>242.51941165526424</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="0"/>
-        <v>93.871760934592928</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64.785496265109373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
-        <v>920</v>
+        <v>1380</v>
       </c>
       <c r="B25">
         <f t="shared" si="2"/>
-        <v>0.92</v>
+        <v>1.38</v>
       </c>
       <c r="C25">
+        <f t="shared" si="3"/>
+        <v>78.799333565611377</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="0"/>
-        <v>63.415921227037977</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19.824222320509609</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
-        <v>960</v>
+        <v>1440</v>
       </c>
       <c r="B26">
         <f t="shared" si="2"/>
-        <v>0.96</v>
+        <v>1.44</v>
       </c>
       <c r="C26">
+        <f t="shared" si="3"/>
+        <v>-149.88523933458049</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="0"/>
-        <v>31.959974558897656</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-35.51197381507555</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="B27">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C27">
+        <f t="shared" si="3"/>
+        <v>-255</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="0"/>
-        <v>3.124128560016981E-14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-56.898190837849604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
-        <v>1040</v>
+        <v>1560</v>
       </c>
       <c r="B28">
         <f t="shared" si="2"/>
-        <v>1.04</v>
+        <v>1.56</v>
       </c>
       <c r="C28">
+        <f t="shared" si="3"/>
+        <v>-149.88523933458086</v>
+      </c>
+      <c r="D28">
         <f t="shared" si="0"/>
-        <v>-31.959974558897478</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-31.496295324755145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
-        <v>1080</v>
+        <v>1620</v>
       </c>
       <c r="B29">
         <f t="shared" si="2"/>
-        <v>1.08</v>
+        <v>1.62</v>
       </c>
       <c r="C29">
+        <f t="shared" si="3"/>
+        <v>78.799333565611789</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="0"/>
-        <v>-63.415921227037913</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15.594285601290384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
-        <v>1120</v>
+        <v>1680</v>
       </c>
       <c r="B30">
         <f t="shared" si="2"/>
-        <v>1.1200000000000001</v>
+        <v>1.68</v>
       </c>
       <c r="C30">
+        <f t="shared" si="3"/>
+        <v>242.51941165526409</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="0"/>
-        <v>-93.871760934592871</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45.199307016929993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
-        <v>1160</v>
+        <v>1740</v>
       </c>
       <c r="B31">
         <f t="shared" si="2"/>
-        <v>1.1599999999999999</v>
+        <v>1.74</v>
       </c>
       <c r="C31">
+        <f t="shared" si="3"/>
+        <v>206.29933356561148</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="0"/>
-        <v>-122.84718689593733</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36.209741674455593</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="B32">
         <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="C32">
+        <f t="shared" si="3"/>
+        <v>2.8117157040152829E-13</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="0"/>
-        <v>-149.88523933458063</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.6477347986890172E-14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
-        <v>1240</v>
+        <v>1860</v>
       </c>
       <c r="B33">
         <f t="shared" si="2"/>
-        <v>1.24</v>
+        <v>1.86</v>
       </c>
       <c r="C33">
+        <f t="shared" si="3"/>
+        <v>-206.29933356561168</v>
+      </c>
+      <c r="D33">
         <f t="shared" si="0"/>
-        <v>-174.55951201181554</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-32.115159899323643</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
-        <v>1280</v>
+        <v>1920</v>
       </c>
       <c r="B34">
         <f t="shared" si="2"/>
-        <v>1.28</v>
+        <v>1.92</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C52" si="3">amplitude*SIN(A34  /omegaTerm)</f>
-        <v>-196.48087690782614</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C34:C52" si="4">amplitude*SIN(A34  /omegaTerm)</f>
+        <v>-242.51941165526426</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:D52" si="5">EXP(Eta*A34)*C34</f>
+        <v>-35.555034200418127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
-        <v>1320</v>
+        <v>1980</v>
       </c>
       <c r="B35">
         <f t="shared" si="2"/>
-        <v>1.32</v>
+        <v>1.98</v>
       </c>
       <c r="C35">
-        <f t="shared" si="3"/>
-        <v>-215.30362100301377</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-78.799333565611462</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="5"/>
+        <v>-10.879763886010611</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
-        <v>1360</v>
+        <v>2040</v>
       </c>
       <c r="B36">
         <f t="shared" si="2"/>
-        <v>1.36</v>
+        <v>2.04</v>
       </c>
       <c r="C36">
-        <f t="shared" si="3"/>
-        <v>-230.73089837883492</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>149.88523933458114</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="5"/>
+        <v>19.489384450379923</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
-        <v>1400</v>
+        <v>2100</v>
       </c>
       <c r="B37">
         <f t="shared" si="2"/>
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="C37">
-        <f t="shared" si="3"/>
-        <v>-242.51941165526415</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>255</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="5"/>
+        <v>31.226389204510387</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
-        <v>1440</v>
+        <v>2160</v>
       </c>
       <c r="B38">
         <f t="shared" si="2"/>
-        <v>1.44</v>
+        <v>2.16</v>
       </c>
       <c r="C38">
-        <f t="shared" si="3"/>
-        <v>-250.48324893581562</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>149.88523933458094</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="5"/>
+        <v>17.285533368079516</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="1"/>
-        <v>1480</v>
+        <v>2220</v>
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>1.48</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="C39">
-        <f t="shared" si="3"/>
-        <v>-254.49681574920925</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-78.799333565612557</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="5"/>
+        <v>-8.558325394561777</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="1"/>
-        <v>1520</v>
+        <v>2280</v>
       </c>
       <c r="B40">
         <f t="shared" si="2"/>
-        <v>1.52</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="C40">
-        <f t="shared" si="3"/>
-        <v>-254.49681574920925</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-242.51941165526432</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="5"/>
+        <v>-24.805905634277575</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="1"/>
-        <v>1560</v>
+        <v>2340</v>
       </c>
       <c r="B41">
         <f t="shared" si="2"/>
-        <v>1.56</v>
+        <v>2.34</v>
       </c>
       <c r="C41">
-        <f t="shared" si="3"/>
-        <v>-250.48324893581562</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-206.29933356561153</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="5"/>
+        <v>-19.872327570900037</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="1"/>
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="C42">
-        <f t="shared" si="3"/>
-        <v>-242.51941165526418</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-3.7489542720203772E-13</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="5"/>
+        <v>-3.4009745853328808E-14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="1"/>
-        <v>1640</v>
+        <v>2460</v>
       </c>
       <c r="B43">
         <f t="shared" si="2"/>
-        <v>1.64</v>
+        <v>2.46</v>
       </c>
       <c r="C43">
-        <f t="shared" si="3"/>
-        <v>-230.73089837883498</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>206.29933356561216</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="5"/>
+        <v>17.625173447769122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="1"/>
-        <v>1680</v>
+        <v>2520</v>
       </c>
       <c r="B44">
         <f t="shared" si="2"/>
-        <v>1.68</v>
+        <v>2.52</v>
       </c>
       <c r="C44">
-        <f t="shared" si="3"/>
-        <v>-215.30362100301394</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>242.51941165526401</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="5"/>
+        <v>19.513016490910516</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="1"/>
-        <v>1720</v>
+        <v>2580</v>
       </c>
       <c r="B45">
         <f t="shared" si="2"/>
-        <v>1.72</v>
+        <v>2.58</v>
       </c>
       <c r="C45">
-        <f t="shared" si="3"/>
-        <v>-196.48087690782634</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>78.799333565611548</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="5"/>
+        <v>5.9709410185981922</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>1760</v>
+        <v>2640</v>
       </c>
       <c r="B46">
         <f t="shared" si="2"/>
-        <v>1.76</v>
+        <v>2.64</v>
       </c>
       <c r="C46">
-        <f t="shared" si="3"/>
-        <v>-174.55951201181568</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-149.88523933458032</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>-10.696000966678424</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>1800</v>
+        <v>2700</v>
       </c>
       <c r="B47">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2.7</v>
       </c>
       <c r="C47">
-        <f t="shared" si="3"/>
-        <v>-149.88523933458072</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-255</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="5"/>
+        <v>-17.137405748636187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>1840</v>
+        <v>2760</v>
       </c>
       <c r="B48">
         <f t="shared" si="2"/>
-        <v>1.84</v>
+        <v>2.76</v>
       </c>
       <c r="C48">
-        <f t="shared" si="3"/>
-        <v>-122.84718689593741</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-149.88523933458026</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="5"/>
+        <v>-9.4865018484935622</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>1880</v>
+        <v>2820</v>
       </c>
       <c r="B49">
         <f t="shared" si="2"/>
-        <v>1.88</v>
+        <v>2.82</v>
       </c>
       <c r="C49">
-        <f t="shared" si="3"/>
-        <v>-93.87176093459307</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>78.799333565611605</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="5"/>
+        <v>4.696908562014448</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>1920</v>
+        <v>2880</v>
       </c>
       <c r="B50">
         <f t="shared" si="2"/>
-        <v>1.92</v>
+        <v>2.88</v>
       </c>
       <c r="C50">
-        <f t="shared" si="3"/>
-        <v>-63.415921227038112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>242.51941165526401</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>13.613769655941891</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>1960</v>
+        <v>2940</v>
       </c>
       <c r="B51">
         <f t="shared" si="2"/>
-        <v>1.96</v>
+        <v>2.94</v>
       </c>
       <c r="C51">
-        <f t="shared" si="3"/>
-        <v>-31.959974558897684</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>206.29933356561105</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="5"/>
+        <v>10.906164607182053</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="B52">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52">
-        <f t="shared" si="3"/>
-        <v>-6.2482571200339621E-14</v>
+        <f t="shared" si="4"/>
+        <v>-4.3732270409158058E-13</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="5"/>
+        <v>-2.1773015367426657E-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest comments/ pinouts or something like that added
</commit_message>
<xml_diff>
--- a/Pins for HoverBoard wheel.xlsx
+++ b/Pins for HoverBoard wheel.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chtacklind\Desktop\git\LMR-QuanumMotor-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7766360-CBF9-4AAB-B138-C919E5ACA143}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29685" windowHeight="16470" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29685" windowHeight="16470" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cables" sheetId="1" r:id="rId1"/>
     <sheet name="Atmel Controler" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId3"/>
-    <sheet name="Truth Table" sheetId="2" r:id="rId4"/>
-    <sheet name="Explore states" sheetId="4" r:id="rId5"/>
-    <sheet name="Sketch" sheetId="3" r:id="rId6"/>
-    <sheet name="3 Hall Synthesis" sheetId="5" r:id="rId7"/>
-    <sheet name="motor test" sheetId="6" r:id="rId8"/>
-    <sheet name="sin Pulse syntesis" sheetId="12" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
+    <sheet name="Truth Table" sheetId="2" r:id="rId3"/>
+    <sheet name="Explore states" sheetId="4" r:id="rId4"/>
+    <sheet name="Sketch" sheetId="3" r:id="rId5"/>
+    <sheet name="3 Hall Synthesis" sheetId="5" r:id="rId6"/>
+    <sheet name="motor test" sheetId="6" r:id="rId7"/>
+    <sheet name="sin Pulse syntesis" sheetId="12" r:id="rId8"/>
+    <sheet name="10 pin" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="amplitude">'sin Pulse syntesis'!$H$2</definedName>
@@ -31,7 +31,7 @@
     <definedName name="omega">'sin Pulse syntesis'!$H$3</definedName>
     <definedName name="omegaTerm">'sin Pulse syntesis'!$H$4</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="295">
   <si>
     <t>Pin out</t>
   </si>
@@ -11509,26 +11509,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29800C5-F2DC-491C-A496-777CBE6FE60C}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B464C57-0DBE-40E5-955E-B8EBE134B27C}">
+  <dimension ref="A1:AD63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B464C57-0DBE-40E5-955E-B8EBE134B27C}">
-  <dimension ref="A1:AB63"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="A24" sqref="A24:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11536,7 +11522,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="62"/>
       <c r="B1" s="63" t="s">
         <v>155</v>
@@ -11583,7 +11569,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="66" t="s">
         <v>233</v>
       </c>
@@ -11651,7 +11637,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>162</v>
       </c>
@@ -11705,7 +11691,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>162</v>
       </c>
@@ -11764,8 +11750,11 @@
       <c r="AB4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="66" t="s">
         <v>162</v>
       </c>
@@ -11824,8 +11813,11 @@
       <c r="AB5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
         <v>162</v>
       </c>
@@ -11886,8 +11878,11 @@
       <c r="AB6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="66" t="s">
         <v>162</v>
       </c>
@@ -11946,8 +11941,11 @@
       <c r="AB7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66" t="s">
         <v>162</v>
       </c>
@@ -12006,8 +12004,11 @@
       <c r="AB8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="66"/>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
@@ -12049,8 +12050,11 @@
         <v>225</v>
       </c>
       <c r="W9" s="58"/>
-    </row>
-    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="66" t="s">
         <v>186</v>
       </c>
@@ -12112,7 +12116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>186</v>
       </c>
@@ -12162,8 +12166,11 @@
         <v>228</v>
       </c>
       <c r="W11" s="58"/>
-    </row>
-    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
         <v>186</v>
       </c>
@@ -12225,7 +12232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66" t="s">
         <v>186</v>
       </c>
@@ -12276,8 +12283,11 @@
       <c r="V13" s="54" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="66"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
@@ -12331,7 +12341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="66" t="s">
         <v>144</v>
       </c>
@@ -12386,7 +12396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
         <v>144</v>
       </c>
@@ -13199,26 +13209,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12C6A90-4194-4CFA-A44E-A9C9B9CC903C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14640,7 +14638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J66"/>
   <sheetViews>
@@ -16883,7 +16881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16898,7 +16896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AT88"/>
   <sheetViews>
@@ -26697,7 +26695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D0068D-F33F-44A4-9DEF-2D0781A661B6}">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -27000,7 +26998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BAE66D-154B-4C32-935A-061D0922E860}">
   <dimension ref="A1:O52"/>
   <sheetViews>
@@ -28006,4 +28004,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29800C5-F2DC-491C-A496-777CBE6FE60C}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>